<commit_message>
acne biomass b2 and b3
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/biomass.xlsx
+++ b/data/treeMeasurements/biomass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0519ACBF-D136-814B-8F8E-D4D9BF51F57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3CEA2B-0D02-3048-AB58-FD86029F880D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -2017,9 +2017,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2479,8 +2480,8 @@
   <dimension ref="A1:I617"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="208" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2538,6 +2539,9 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="G2">
+        <v>304</v>
+      </c>
       <c r="H2">
         <v>6.1</v>
       </c>
@@ -2561,6 +2565,9 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="G3">
+        <v>304</v>
+      </c>
       <c r="H3">
         <v>6.4</v>
       </c>
@@ -2584,6 +2591,9 @@
       <c r="E4" t="s">
         <v>9</v>
       </c>
+      <c r="G4">
+        <v>304</v>
+      </c>
       <c r="H4">
         <v>11.4</v>
       </c>
@@ -2607,6 +2617,9 @@
       <c r="E5" t="s">
         <v>9</v>
       </c>
+      <c r="G5">
+        <v>304</v>
+      </c>
       <c r="H5">
         <v>7.6</v>
       </c>
@@ -2630,6 +2643,9 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
+      <c r="G6">
+        <v>304</v>
+      </c>
       <c r="H6">
         <v>13.4</v>
       </c>
@@ -2653,6 +2669,15 @@
       <c r="E7" t="s">
         <v>9</v>
       </c>
+      <c r="G7">
+        <v>307</v>
+      </c>
+      <c r="H7">
+        <v>12.54</v>
+      </c>
+      <c r="I7">
+        <v>23.18</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -2670,6 +2695,15 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
+      <c r="G8">
+        <v>307</v>
+      </c>
+      <c r="H8">
+        <v>7.41</v>
+      </c>
+      <c r="I8">
+        <v>13.67</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -2687,6 +2721,15 @@
       <c r="E9" t="s">
         <v>9</v>
       </c>
+      <c r="G9">
+        <v>307</v>
+      </c>
+      <c r="H9">
+        <v>13.37</v>
+      </c>
+      <c r="I9">
+        <v>16.239999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -2704,6 +2747,15 @@
       <c r="E10" t="s">
         <v>9</v>
       </c>
+      <c r="G10">
+        <v>307</v>
+      </c>
+      <c r="H10">
+        <v>12.53</v>
+      </c>
+      <c r="I10">
+        <v>18.260000000000002</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2721,6 +2773,15 @@
       <c r="E11" t="s">
         <v>9</v>
       </c>
+      <c r="G11">
+        <v>307</v>
+      </c>
+      <c r="H11">
+        <v>8.0299999999999994</v>
+      </c>
+      <c r="I11">
+        <v>14.04</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -2738,6 +2799,15 @@
       <c r="E12" t="s">
         <v>9</v>
       </c>
+      <c r="G12">
+        <v>307</v>
+      </c>
+      <c r="H12">
+        <v>7.85</v>
+      </c>
+      <c r="I12">
+        <v>8.67</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2755,6 +2825,15 @@
       <c r="E13" t="s">
         <v>9</v>
       </c>
+      <c r="G13">
+        <v>307</v>
+      </c>
+      <c r="H13">
+        <v>3.83</v>
+      </c>
+      <c r="I13">
+        <v>4.1399999999999997</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -2772,6 +2851,15 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
+      <c r="G14">
+        <v>307</v>
+      </c>
+      <c r="H14">
+        <v>5.31</v>
+      </c>
+      <c r="I14">
+        <v>8.39</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -2789,6 +2877,15 @@
       <c r="E15" t="s">
         <v>9</v>
       </c>
+      <c r="G15">
+        <v>307</v>
+      </c>
+      <c r="H15">
+        <v>6.02</v>
+      </c>
+      <c r="I15">
+        <v>9.85</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -2806,6 +2903,15 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
+      <c r="G16">
+        <v>307</v>
+      </c>
+      <c r="H16">
+        <v>7.24</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -2823,6 +2929,9 @@
       <c r="E17" t="s">
         <v>9</v>
       </c>
+      <c r="G17">
+        <v>304</v>
+      </c>
       <c r="H17">
         <v>11.5</v>
       </c>
@@ -2846,6 +2955,9 @@
       <c r="E18" t="s">
         <v>9</v>
       </c>
+      <c r="G18">
+        <v>304</v>
+      </c>
       <c r="H18">
         <v>9.6999999999999993</v>
       </c>
@@ -2869,6 +2981,9 @@
       <c r="E19" t="s">
         <v>9</v>
       </c>
+      <c r="G19">
+        <v>304</v>
+      </c>
       <c r="H19">
         <v>7.2</v>
       </c>
@@ -2892,6 +3007,9 @@
       <c r="E20" t="s">
         <v>9</v>
       </c>
+      <c r="G20">
+        <v>304</v>
+      </c>
       <c r="H20">
         <v>10.4</v>
       </c>
@@ -2915,6 +3033,9 @@
       <c r="E21" t="s">
         <v>9</v>
       </c>
+      <c r="G21">
+        <v>304</v>
+      </c>
       <c r="H21">
         <v>5.97</v>
       </c>
@@ -2938,6 +3059,15 @@
       <c r="E22" t="s">
         <v>9</v>
       </c>
+      <c r="G22">
+        <v>307</v>
+      </c>
+      <c r="H22">
+        <v>11.73</v>
+      </c>
+      <c r="I22">
+        <v>17.13</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -2955,6 +3085,15 @@
       <c r="E23" t="s">
         <v>9</v>
       </c>
+      <c r="G23">
+        <v>307</v>
+      </c>
+      <c r="H23">
+        <v>10.56</v>
+      </c>
+      <c r="I23">
+        <v>18.71</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2972,6 +3111,15 @@
       <c r="E24" t="s">
         <v>9</v>
       </c>
+      <c r="G24">
+        <v>307</v>
+      </c>
+      <c r="H24">
+        <v>4.2</v>
+      </c>
+      <c r="I24">
+        <v>5.98</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -2989,6 +3137,15 @@
       <c r="E25" t="s">
         <v>9</v>
       </c>
+      <c r="G25">
+        <v>307</v>
+      </c>
+      <c r="H25">
+        <v>12.74</v>
+      </c>
+      <c r="I25">
+        <v>15.02</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
@@ -3006,6 +3163,15 @@
       <c r="E26" t="s">
         <v>9</v>
       </c>
+      <c r="G26">
+        <v>307</v>
+      </c>
+      <c r="H26">
+        <v>9.1</v>
+      </c>
+      <c r="I26">
+        <v>13.75</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
@@ -3023,6 +3189,15 @@
       <c r="E27" t="s">
         <v>9</v>
       </c>
+      <c r="G27">
+        <v>307</v>
+      </c>
+      <c r="H27">
+        <v>7.09</v>
+      </c>
+      <c r="I27">
+        <v>7.72</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -3040,6 +3215,15 @@
       <c r="E28" t="s">
         <v>9</v>
       </c>
+      <c r="G28">
+        <v>307</v>
+      </c>
+      <c r="H28">
+        <v>7.39</v>
+      </c>
+      <c r="I28">
+        <v>10.43</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
@@ -3057,6 +3241,15 @@
       <c r="E29" t="s">
         <v>9</v>
       </c>
+      <c r="G29">
+        <v>307</v>
+      </c>
+      <c r="H29">
+        <v>5.86</v>
+      </c>
+      <c r="I29">
+        <v>5.34</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -3074,6 +3267,15 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
+      <c r="G30">
+        <v>307</v>
+      </c>
+      <c r="H30">
+        <v>6.6</v>
+      </c>
+      <c r="I30">
+        <v>9.43</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -3091,6 +3293,15 @@
       <c r="E31" t="s">
         <v>9</v>
       </c>
+      <c r="G31">
+        <v>307</v>
+      </c>
+      <c r="H31" s="2">
+        <v>7.14</v>
+      </c>
+      <c r="I31" s="2">
+        <v>7.79</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -3108,6 +3319,9 @@
       <c r="E32" t="s">
         <v>9</v>
       </c>
+      <c r="G32">
+        <v>304</v>
+      </c>
       <c r="H32">
         <v>5.78</v>
       </c>
@@ -3131,6 +3345,9 @@
       <c r="E33" t="s">
         <v>9</v>
       </c>
+      <c r="G33">
+        <v>304</v>
+      </c>
       <c r="H33">
         <v>7.96</v>
       </c>
@@ -3154,6 +3371,9 @@
       <c r="E34" t="s">
         <v>9</v>
       </c>
+      <c r="G34">
+        <v>304</v>
+      </c>
       <c r="H34">
         <v>5.22</v>
       </c>
@@ -3177,6 +3397,9 @@
       <c r="E35" t="s">
         <v>9</v>
       </c>
+      <c r="G35">
+        <v>304</v>
+      </c>
       <c r="H35">
         <v>7.06</v>
       </c>
@@ -3200,6 +3423,9 @@
       <c r="E36" t="s">
         <v>9</v>
       </c>
+      <c r="G36">
+        <v>304</v>
+      </c>
       <c r="H36">
         <v>6.08</v>
       </c>
@@ -3223,6 +3449,15 @@
       <c r="E37" t="s">
         <v>9</v>
       </c>
+      <c r="G37">
+        <v>307</v>
+      </c>
+      <c r="H37">
+        <v>6.36</v>
+      </c>
+      <c r="I37">
+        <v>12.25</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -3240,6 +3475,15 @@
       <c r="E38" t="s">
         <v>9</v>
       </c>
+      <c r="G38">
+        <v>307</v>
+      </c>
+      <c r="H38">
+        <v>7.35</v>
+      </c>
+      <c r="I38">
+        <v>12.86</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
@@ -3257,6 +3501,15 @@
       <c r="E39" t="s">
         <v>9</v>
       </c>
+      <c r="G39">
+        <v>307</v>
+      </c>
+      <c r="H39">
+        <v>9.35</v>
+      </c>
+      <c r="I39">
+        <v>15.66</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -3274,6 +3527,15 @@
       <c r="E40" t="s">
         <v>9</v>
       </c>
+      <c r="G40">
+        <v>307</v>
+      </c>
+      <c r="H40">
+        <v>7.33</v>
+      </c>
+      <c r="I40">
+        <v>12.93</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -3291,6 +3553,15 @@
       <c r="E41" t="s">
         <v>9</v>
       </c>
+      <c r="G41">
+        <v>307</v>
+      </c>
+      <c r="H41">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="I41">
+        <v>5.6</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
@@ -3308,6 +3579,15 @@
       <c r="E42" t="s">
         <v>9</v>
       </c>
+      <c r="G42">
+        <v>307</v>
+      </c>
+      <c r="H42">
+        <v>10.15</v>
+      </c>
+      <c r="I42">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
@@ -3325,6 +3605,15 @@
       <c r="E43" t="s">
         <v>9</v>
       </c>
+      <c r="G43">
+        <v>307</v>
+      </c>
+      <c r="H43">
+        <v>2.09</v>
+      </c>
+      <c r="I43">
+        <v>3.07</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
@@ -3342,6 +3631,15 @@
       <c r="E44" t="s">
         <v>9</v>
       </c>
+      <c r="G44">
+        <v>307</v>
+      </c>
+      <c r="H44">
+        <v>11.51</v>
+      </c>
+      <c r="I44">
+        <v>17.28</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
@@ -3359,6 +3657,15 @@
       <c r="E45" t="s">
         <v>9</v>
       </c>
+      <c r="G45">
+        <v>307</v>
+      </c>
+      <c r="H45">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="I45">
+        <v>9.2200000000000006</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
@@ -3376,6 +3683,15 @@
       <c r="E46" t="s">
         <v>9</v>
       </c>
+      <c r="G46">
+        <v>307</v>
+      </c>
+      <c r="H46">
+        <v>5.67</v>
+      </c>
+      <c r="I46">
+        <v>13.38</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -3393,6 +3709,9 @@
       <c r="E47" t="s">
         <v>9</v>
       </c>
+      <c r="G47">
+        <v>304</v>
+      </c>
       <c r="H47">
         <v>9.92</v>
       </c>
@@ -3416,6 +3735,9 @@
       <c r="E48" t="s">
         <v>9</v>
       </c>
+      <c r="G48">
+        <v>304</v>
+      </c>
       <c r="H48">
         <v>5.72</v>
       </c>
@@ -3439,6 +3761,9 @@
       <c r="E49" t="s">
         <v>9</v>
       </c>
+      <c r="G49">
+        <v>304</v>
+      </c>
       <c r="H49">
         <v>12.11</v>
       </c>
@@ -3462,6 +3787,9 @@
       <c r="E50" t="s">
         <v>9</v>
       </c>
+      <c r="G50">
+        <v>304</v>
+      </c>
       <c r="H50">
         <v>10.55</v>
       </c>
@@ -3485,6 +3813,9 @@
       <c r="E51" t="s">
         <v>9</v>
       </c>
+      <c r="G51">
+        <v>304</v>
+      </c>
       <c r="H51">
         <v>8.44</v>
       </c>
@@ -3508,6 +3839,15 @@
       <c r="E52" t="s">
         <v>9</v>
       </c>
+      <c r="G52">
+        <v>307</v>
+      </c>
+      <c r="H52">
+        <v>5.27</v>
+      </c>
+      <c r="I52">
+        <v>8.86</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
@@ -3525,6 +3865,15 @@
       <c r="E53" t="s">
         <v>9</v>
       </c>
+      <c r="G53">
+        <v>307</v>
+      </c>
+      <c r="H53">
+        <v>11.38</v>
+      </c>
+      <c r="I53">
+        <v>17.61</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
@@ -3542,6 +3891,15 @@
       <c r="E54" t="s">
         <v>9</v>
       </c>
+      <c r="G54">
+        <v>307</v>
+      </c>
+      <c r="H54">
+        <v>12.75</v>
+      </c>
+      <c r="I54">
+        <v>26.02</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -3559,6 +3917,15 @@
       <c r="E55" t="s">
         <v>9</v>
       </c>
+      <c r="G55">
+        <v>307</v>
+      </c>
+      <c r="H55">
+        <v>7.53</v>
+      </c>
+      <c r="I55">
+        <v>7.82</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
@@ -3576,6 +3943,15 @@
       <c r="E56" t="s">
         <v>9</v>
       </c>
+      <c r="G56">
+        <v>307</v>
+      </c>
+      <c r="H56">
+        <v>5.86</v>
+      </c>
+      <c r="I56">
+        <v>8.51</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
@@ -3593,6 +3969,15 @@
       <c r="E57" t="s">
         <v>9</v>
       </c>
+      <c r="G57">
+        <v>307</v>
+      </c>
+      <c r="H57">
+        <v>7.46</v>
+      </c>
+      <c r="I57">
+        <v>9.7899999999999991</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
@@ -3610,6 +3995,15 @@
       <c r="E58" t="s">
         <v>9</v>
       </c>
+      <c r="G58">
+        <v>307</v>
+      </c>
+      <c r="H58">
+        <v>12.27</v>
+      </c>
+      <c r="I58">
+        <v>13.92</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
@@ -3627,6 +4021,15 @@
       <c r="E59" t="s">
         <v>9</v>
       </c>
+      <c r="G59">
+        <v>307</v>
+      </c>
+      <c r="H59">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="I59">
+        <v>28.77</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
@@ -3644,6 +4047,15 @@
       <c r="E60" t="s">
         <v>9</v>
       </c>
+      <c r="G60">
+        <v>307</v>
+      </c>
+      <c r="H60">
+        <v>5.42</v>
+      </c>
+      <c r="I60">
+        <v>7.72</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
@@ -3661,6 +4073,15 @@
       <c r="E61" t="s">
         <v>9</v>
       </c>
+      <c r="G61">
+        <v>307</v>
+      </c>
+      <c r="H61">
+        <v>8.19</v>
+      </c>
+      <c r="I61">
+        <v>10.32</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -3678,6 +4099,9 @@
       <c r="E62" t="s">
         <v>9</v>
       </c>
+      <c r="G62">
+        <v>304</v>
+      </c>
       <c r="H62">
         <v>5.32</v>
       </c>
@@ -3701,6 +4125,9 @@
       <c r="E63" t="s">
         <v>9</v>
       </c>
+      <c r="G63">
+        <v>304</v>
+      </c>
       <c r="H63">
         <v>5.17</v>
       </c>
@@ -3724,6 +4151,9 @@
       <c r="E64" t="s">
         <v>9</v>
       </c>
+      <c r="G64">
+        <v>304</v>
+      </c>
       <c r="H64">
         <v>6.49</v>
       </c>
@@ -3747,6 +4177,9 @@
       <c r="E65" t="s">
         <v>9</v>
       </c>
+      <c r="G65">
+        <v>304</v>
+      </c>
       <c r="H65">
         <v>3.14</v>
       </c>
@@ -3770,6 +4203,9 @@
       <c r="E66" t="s">
         <v>9</v>
       </c>
+      <c r="G66">
+        <v>304</v>
+      </c>
       <c r="H66">
         <v>10.86</v>
       </c>
@@ -3793,6 +4229,15 @@
       <c r="E67" t="s">
         <v>9</v>
       </c>
+      <c r="G67">
+        <v>307</v>
+      </c>
+      <c r="H67">
+        <v>6.1</v>
+      </c>
+      <c r="I67">
+        <v>11.66</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -3810,6 +4255,15 @@
       <c r="E68" t="s">
         <v>9</v>
       </c>
+      <c r="G68">
+        <v>307</v>
+      </c>
+      <c r="H68">
+        <v>8.14</v>
+      </c>
+      <c r="I68">
+        <v>14.84</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -3827,6 +4281,15 @@
       <c r="E69" t="s">
         <v>9</v>
       </c>
+      <c r="G69">
+        <v>307</v>
+      </c>
+      <c r="H69">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="I69">
+        <v>20.25</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
@@ -3844,6 +4307,15 @@
       <c r="E70" t="s">
         <v>9</v>
       </c>
+      <c r="G70">
+        <v>307</v>
+      </c>
+      <c r="H70">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="I70">
+        <v>14.89</v>
+      </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
@@ -3861,6 +4333,15 @@
       <c r="E71" t="s">
         <v>9</v>
       </c>
+      <c r="G71">
+        <v>307</v>
+      </c>
+      <c r="H71">
+        <v>7.72</v>
+      </c>
+      <c r="I71">
+        <v>13.77</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -3878,6 +4359,15 @@
       <c r="E72" t="s">
         <v>9</v>
       </c>
+      <c r="G72">
+        <v>307</v>
+      </c>
+      <c r="H72">
+        <v>7.32</v>
+      </c>
+      <c r="I72">
+        <v>10.75</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
@@ -3895,6 +4385,15 @@
       <c r="E73" t="s">
         <v>9</v>
       </c>
+      <c r="G73">
+        <v>307</v>
+      </c>
+      <c r="H73">
+        <v>8.61</v>
+      </c>
+      <c r="I73">
+        <v>13.33</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
@@ -3912,6 +4411,15 @@
       <c r="E74" t="s">
         <v>9</v>
       </c>
+      <c r="G74">
+        <v>307</v>
+      </c>
+      <c r="H74">
+        <v>7.12</v>
+      </c>
+      <c r="I74">
+        <v>12.44</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
@@ -3929,6 +4437,15 @@
       <c r="E75" t="s">
         <v>9</v>
       </c>
+      <c r="G75">
+        <v>307</v>
+      </c>
+      <c r="H75">
+        <v>6.25</v>
+      </c>
+      <c r="I75">
+        <v>10.7</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
@@ -3946,6 +4463,15 @@
       <c r="E76" t="s">
         <v>9</v>
       </c>
+      <c r="G76">
+        <v>307</v>
+      </c>
+      <c r="H76">
+        <v>6.38</v>
+      </c>
+      <c r="I76">
+        <v>6.24</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
@@ -3963,6 +4489,9 @@
       <c r="E77" t="s">
         <v>9</v>
       </c>
+      <c r="G77">
+        <v>304</v>
+      </c>
       <c r="H77">
         <v>5.46</v>
       </c>
@@ -3986,6 +4515,9 @@
       <c r="E78" t="s">
         <v>9</v>
       </c>
+      <c r="G78">
+        <v>304</v>
+      </c>
       <c r="H78">
         <v>8.1199999999999992</v>
       </c>
@@ -4009,6 +4541,9 @@
       <c r="E79" t="s">
         <v>9</v>
       </c>
+      <c r="G79">
+        <v>304</v>
+      </c>
       <c r="H79">
         <v>5.03</v>
       </c>
@@ -4032,6 +4567,9 @@
       <c r="E80" t="s">
         <v>9</v>
       </c>
+      <c r="G80">
+        <v>304</v>
+      </c>
       <c r="H80">
         <v>2.96</v>
       </c>
@@ -4055,6 +4593,9 @@
       <c r="E81" t="s">
         <v>9</v>
       </c>
+      <c r="G81">
+        <v>304</v>
+      </c>
       <c r="H81">
         <v>5.38</v>
       </c>
@@ -4078,6 +4619,15 @@
       <c r="E82" t="s">
         <v>9</v>
       </c>
+      <c r="G82">
+        <v>307</v>
+      </c>
+      <c r="H82">
+        <v>8</v>
+      </c>
+      <c r="I82">
+        <v>13.24</v>
+      </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
@@ -4095,6 +4645,15 @@
       <c r="E83" t="s">
         <v>9</v>
       </c>
+      <c r="G83">
+        <v>307</v>
+      </c>
+      <c r="H83">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="I83">
+        <v>13.37</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
@@ -4112,6 +4671,15 @@
       <c r="E84" t="s">
         <v>9</v>
       </c>
+      <c r="G84">
+        <v>307</v>
+      </c>
+      <c r="H84">
+        <v>12.42</v>
+      </c>
+      <c r="I84">
+        <v>18.36</v>
+      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -4129,6 +4697,15 @@
       <c r="E85" t="s">
         <v>9</v>
       </c>
+      <c r="G85">
+        <v>307</v>
+      </c>
+      <c r="H85">
+        <v>4.78</v>
+      </c>
+      <c r="I85">
+        <v>6.97</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -4146,6 +4723,15 @@
       <c r="E86" t="s">
         <v>9</v>
       </c>
+      <c r="G86">
+        <v>307</v>
+      </c>
+      <c r="H86">
+        <v>9.67</v>
+      </c>
+      <c r="I86">
+        <v>17.399999999999999</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
@@ -4163,6 +4749,15 @@
       <c r="E87" t="s">
         <v>9</v>
       </c>
+      <c r="G87">
+        <v>307</v>
+      </c>
+      <c r="H87">
+        <v>6.66</v>
+      </c>
+      <c r="I87">
+        <v>14.07</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -4180,6 +4775,15 @@
       <c r="E88" t="s">
         <v>9</v>
       </c>
+      <c r="G88">
+        <v>307</v>
+      </c>
+      <c r="H88">
+        <v>12.56</v>
+      </c>
+      <c r="I88">
+        <v>11.56</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -4197,6 +4801,15 @@
       <c r="E89" t="s">
         <v>9</v>
       </c>
+      <c r="G89">
+        <v>307</v>
+      </c>
+      <c r="H89">
+        <v>11.81</v>
+      </c>
+      <c r="I89">
+        <v>21.69</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
@@ -4214,6 +4827,15 @@
       <c r="E90" t="s">
         <v>9</v>
       </c>
+      <c r="G90">
+        <v>307</v>
+      </c>
+      <c r="H90">
+        <v>5.51</v>
+      </c>
+      <c r="I90">
+        <v>13.22</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
@@ -4230,6 +4852,15 @@
       </c>
       <c r="E91" t="s">
         <v>9</v>
+      </c>
+      <c r="G91">
+        <v>307</v>
+      </c>
+      <c r="H91">
+        <v>12.04</v>
+      </c>
+      <c r="I91">
+        <v>17.54</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
biomass quma B1 and B2
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/biomass.xlsx
+++ b/data/treeMeasurements/biomass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DBE017-2EAE-3C44-8C67-15DEC368C438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C95581-CCC3-CB42-B9B3-24CFCD79183B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2476" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2480" uniqueCount="648">
   <si>
     <t>tree_ID</t>
   </si>
@@ -1977,6 +1977,9 @@
   </si>
   <si>
     <t>dead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -2026,7 +2029,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2102,7 +2105,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>357</xdr:row>
+      <xdr:row>437</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2190,9 +2193,14 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I617" totalsRowShown="0">
   <autoFilter ref="A1:I617" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="prunus_virginiana"/>
+        <filter val="quercus_macrocarpa"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2489,11 +2497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I617"/>
+  <dimension ref="A1:J617"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J430" sqref="J430"/>
+      <selection pane="topRight" activeCell="J456" sqref="J456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2502,7 +2510,7 @@
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.6640625" customWidth="1"/>
     <col min="6" max="6" width="18.1640625" customWidth="1"/>
-    <col min="7" max="7" width="3" customWidth="1"/>
+    <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" customWidth="1"/>
     <col min="9" max="10" width="19.33203125" customWidth="1"/>
   </cols>
@@ -9399,7 +9407,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>376</v>
       </c>
@@ -9422,7 +9430,7 @@
         <v>18.43</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>379</v>
       </c>
@@ -9445,7 +9453,7 @@
         <v>11.69</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>380</v>
       </c>
@@ -9468,7 +9476,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>381</v>
       </c>
@@ -9491,7 +9499,7 @@
         <v>10.77</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>382</v>
       </c>
@@ -9514,7 +9522,7 @@
         <v>11.86</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>383</v>
       </c>
@@ -9537,7 +9545,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>384</v>
       </c>
@@ -9560,7 +9568,7 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>385</v>
       </c>
@@ -9583,7 +9591,7 @@
         <v>7.55</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>386</v>
       </c>
@@ -9606,7 +9614,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>387</v>
       </c>
@@ -9629,7 +9637,7 @@
         <v>10.74</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>388</v>
       </c>
@@ -9652,7 +9660,7 @@
         <v>7.15</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>389</v>
       </c>
@@ -9675,7 +9683,7 @@
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>390</v>
       </c>
@@ -9698,7 +9706,7 @@
         <v>4.32</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>391</v>
       </c>
@@ -9721,7 +9729,7 @@
         <v>3.51</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>392</v>
       </c>
@@ -9744,7 +9752,7 @@
         <v>8.7899999999999991</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>393</v>
       </c>
@@ -9767,7 +9775,7 @@
         <v>17.47</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>394</v>
       </c>
@@ -9790,7 +9798,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>395</v>
       </c>
@@ -9813,7 +9821,7 @@
         <v>7.44</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>396</v>
       </c>
@@ -9836,7 +9844,7 @@
         <v>14.15</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>397</v>
       </c>
@@ -9859,7 +9867,7 @@
         <v>11.47</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>398</v>
       </c>
@@ -9882,7 +9890,7 @@
         <v>15.58</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>399</v>
       </c>
@@ -9905,7 +9913,7 @@
         <v>14.61</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>400</v>
       </c>
@@ -9928,7 +9936,7 @@
         <v>13.12</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>401</v>
       </c>
@@ -9951,7 +9959,7 @@
         <v>12.64</v>
       </c>
     </row>
-    <row r="382" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>402</v>
       </c>
@@ -9974,7 +9982,7 @@
         <v>4.1900000000000004</v>
       </c>
     </row>
-    <row r="383" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>403</v>
       </c>
@@ -9997,7 +10005,7 @@
         <v>12.71</v>
       </c>
     </row>
-    <row r="384" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>404</v>
       </c>
@@ -10020,7 +10028,7 @@
         <v>12.69</v>
       </c>
     </row>
-    <row r="385" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>405</v>
       </c>
@@ -10043,7 +10051,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="386" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>406</v>
       </c>
@@ -10066,7 +10074,7 @@
         <v>12.64</v>
       </c>
     </row>
-    <row r="387" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>407</v>
       </c>
@@ -10089,7 +10097,7 @@
         <v>6.03</v>
       </c>
     </row>
-    <row r="388" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>408</v>
       </c>
@@ -10112,7 +10120,7 @@
         <v>17.350000000000001</v>
       </c>
     </row>
-    <row r="389" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>409</v>
       </c>
@@ -10135,7 +10143,7 @@
         <v>13.63</v>
       </c>
     </row>
-    <row r="390" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>410</v>
       </c>
@@ -10158,7 +10166,7 @@
         <v>14.28</v>
       </c>
     </row>
-    <row r="391" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>411</v>
       </c>
@@ -10181,7 +10189,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="392" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>412</v>
       </c>
@@ -10204,7 +10212,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="393" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>413</v>
       </c>
@@ -10227,7 +10235,7 @@
         <v>15.76</v>
       </c>
     </row>
-    <row r="394" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>414</v>
       </c>
@@ -10250,7 +10258,7 @@
         <v>10.220000000000001</v>
       </c>
     </row>
-    <row r="395" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>415</v>
       </c>
@@ -10273,7 +10281,7 @@
         <v>8.1300000000000008</v>
       </c>
     </row>
-    <row r="396" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>416</v>
       </c>
@@ -10296,7 +10304,7 @@
         <v>9.2899999999999991</v>
       </c>
     </row>
-    <row r="397" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>417</v>
       </c>
@@ -10319,7 +10327,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="398" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>418</v>
       </c>
@@ -10342,7 +10350,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="399" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>419</v>
       </c>
@@ -10365,7 +10373,7 @@
         <v>6.39</v>
       </c>
     </row>
-    <row r="400" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>420</v>
       </c>
@@ -10381,14 +10389,14 @@
       <c r="E400" t="s">
         <v>378</v>
       </c>
-      <c r="H400" s="2">
+      <c r="H400">
         <v>1.65</v>
       </c>
-      <c r="I400" s="2">
+      <c r="I400">
         <v>11.44</v>
       </c>
     </row>
-    <row r="401" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>421</v>
       </c>
@@ -10411,7 +10419,7 @@
         <v>12.66</v>
       </c>
     </row>
-    <row r="402" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>422</v>
       </c>
@@ -10434,7 +10442,7 @@
         <v>14.87</v>
       </c>
     </row>
-    <row r="403" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>423</v>
       </c>
@@ -10457,7 +10465,7 @@
         <v>10.71</v>
       </c>
     </row>
-    <row r="404" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>424</v>
       </c>
@@ -10480,7 +10488,7 @@
         <v>20.76</v>
       </c>
     </row>
-    <row r="405" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>425</v>
       </c>
@@ -10503,7 +10511,7 @@
         <v>18.649999999999999</v>
       </c>
     </row>
-    <row r="406" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>426</v>
       </c>
@@ -10526,7 +10534,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="407" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>427</v>
       </c>
@@ -10549,7 +10557,7 @@
         <v>11.58</v>
       </c>
     </row>
-    <row r="408" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>428</v>
       </c>
@@ -10572,7 +10580,7 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="409" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>429</v>
       </c>
@@ -10595,7 +10603,7 @@
         <v>14.87</v>
       </c>
     </row>
-    <row r="410" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>430</v>
       </c>
@@ -10618,7 +10626,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="411" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>431</v>
       </c>
@@ -10641,7 +10649,7 @@
         <v>11.04</v>
       </c>
     </row>
-    <row r="412" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>432</v>
       </c>
@@ -10664,7 +10672,7 @@
         <v>13.15</v>
       </c>
     </row>
-    <row r="413" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>433</v>
       </c>
@@ -10687,7 +10695,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="414" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>434</v>
       </c>
@@ -10710,7 +10718,7 @@
         <v>8.11</v>
       </c>
     </row>
-    <row r="415" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>435</v>
       </c>
@@ -10733,7 +10741,7 @@
         <v>20.05</v>
       </c>
     </row>
-    <row r="416" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>436</v>
       </c>
@@ -10756,7 +10764,7 @@
         <v>16.37</v>
       </c>
     </row>
-    <row r="417" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>437</v>
       </c>
@@ -10779,7 +10787,7 @@
         <v>6.99</v>
       </c>
     </row>
-    <row r="418" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>438</v>
       </c>
@@ -10802,7 +10810,7 @@
         <v>22.44</v>
       </c>
     </row>
-    <row r="419" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>439</v>
       </c>
@@ -10825,7 +10833,7 @@
         <v>12.02</v>
       </c>
     </row>
-    <row r="420" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>440</v>
       </c>
@@ -10848,7 +10856,7 @@
         <v>9.94</v>
       </c>
     </row>
-    <row r="421" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>441</v>
       </c>
@@ -10871,7 +10879,7 @@
         <v>7.93</v>
       </c>
     </row>
-    <row r="422" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>442</v>
       </c>
@@ -10894,7 +10902,7 @@
         <v>16.63</v>
       </c>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>443</v>
       </c>
@@ -10917,7 +10925,7 @@
         <v>9.5500000000000007</v>
       </c>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>444</v>
       </c>
@@ -10940,7 +10948,7 @@
         <v>11.43</v>
       </c>
     </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>445</v>
       </c>
@@ -10963,7 +10971,7 @@
         <v>9.3000000000000007</v>
       </c>
     </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>446</v>
       </c>
@@ -10986,7 +10994,7 @@
         <v>11.47</v>
       </c>
     </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>447</v>
       </c>
@@ -11009,7 +11017,7 @@
         <v>12.93</v>
       </c>
     </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>448</v>
       </c>
@@ -11032,7 +11040,7 @@
         <v>18.88</v>
       </c>
     </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>449</v>
       </c>
@@ -11055,7 +11063,7 @@
         <v>12.62</v>
       </c>
     </row>
-    <row r="430" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>450</v>
       </c>
@@ -11078,7 +11086,7 @@
         <v>13.81</v>
       </c>
     </row>
-    <row r="431" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
         <v>451</v>
       </c>
@@ -11101,7 +11109,7 @@
         <v>5.31</v>
       </c>
     </row>
-    <row r="432" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432" t="s">
         <v>452</v>
       </c>
@@ -11124,7 +11132,7 @@
         <v>16.78</v>
       </c>
     </row>
-    <row r="433" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
         <v>453</v>
       </c>
@@ -11147,7 +11155,7 @@
         <v>12.52</v>
       </c>
     </row>
-    <row r="434" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434" t="s">
         <v>454</v>
       </c>
@@ -11170,7 +11178,7 @@
         <v>22.46</v>
       </c>
     </row>
-    <row r="435" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A435" t="s">
         <v>455</v>
       </c>
@@ -11193,7 +11201,7 @@
         <v>12.67</v>
       </c>
     </row>
-    <row r="436" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436" t="s">
         <v>456</v>
       </c>
@@ -11216,7 +11224,7 @@
         <v>6.77</v>
       </c>
     </row>
-    <row r="437" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437" t="s">
         <v>457</v>
       </c>
@@ -11239,7 +11247,7 @@
         <v>5.71</v>
       </c>
     </row>
-    <row r="438" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A438" t="s">
         <v>458</v>
       </c>
@@ -11255,8 +11263,14 @@
       <c r="E438" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="439" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H438">
+        <v>11.08</v>
+      </c>
+      <c r="I438">
+        <v>54.12</v>
+      </c>
+    </row>
+    <row r="439" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A439" t="s">
         <v>461</v>
       </c>
@@ -11272,8 +11286,14 @@
       <c r="E439" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H439">
+        <v>12.01</v>
+      </c>
+      <c r="I439">
+        <v>33.42</v>
+      </c>
+    </row>
+    <row r="440" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A440" t="s">
         <v>462</v>
       </c>
@@ -11289,8 +11309,14 @@
       <c r="E440" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="441" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H440">
+        <v>8.85</v>
+      </c>
+      <c r="I440">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="441" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A441" t="s">
         <v>463</v>
       </c>
@@ -11306,8 +11332,14 @@
       <c r="E441" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H441">
+        <v>13.94</v>
+      </c>
+      <c r="I441">
+        <v>61.33</v>
+      </c>
+    </row>
+    <row r="442" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A442" t="s">
         <v>464</v>
       </c>
@@ -11322,6 +11354,12 @@
       </c>
       <c r="E442" t="s">
         <v>460</v>
+      </c>
+      <c r="H442">
+        <v>6.5</v>
+      </c>
+      <c r="I442">
+        <v>32.15</v>
       </c>
     </row>
     <row r="443" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -11340,6 +11378,15 @@
       <c r="E443" t="s">
         <v>460</v>
       </c>
+      <c r="G443">
+        <v>321</v>
+      </c>
+      <c r="H443">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="I443">
+        <v>56.55</v>
+      </c>
     </row>
     <row r="444" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A444" t="s">
@@ -11357,6 +11404,12 @@
       <c r="E444" t="s">
         <v>460</v>
       </c>
+      <c r="H444">
+        <v>15.35</v>
+      </c>
+      <c r="I444">
+        <v>49.34</v>
+      </c>
     </row>
     <row r="445" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445" t="s">
@@ -11374,6 +11427,12 @@
       <c r="E445" t="s">
         <v>460</v>
       </c>
+      <c r="H445">
+        <v>14.16</v>
+      </c>
+      <c r="I445">
+        <v>45.27</v>
+      </c>
     </row>
     <row r="446" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446" t="s">
@@ -11391,6 +11450,12 @@
       <c r="E446" t="s">
         <v>460</v>
       </c>
+      <c r="H446">
+        <v>5.65</v>
+      </c>
+      <c r="I446">
+        <v>24.37</v>
+      </c>
     </row>
     <row r="447" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447" t="s">
@@ -11408,6 +11473,12 @@
       <c r="E447" t="s">
         <v>460</v>
       </c>
+      <c r="H447">
+        <v>12.78</v>
+      </c>
+      <c r="I447">
+        <v>42.59</v>
+      </c>
     </row>
     <row r="448" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448" t="s">
@@ -11435,7 +11506,7 @@
         <v>39.729999999999997</v>
       </c>
     </row>
-    <row r="449" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" t="s">
         <v>471</v>
       </c>
@@ -11461,7 +11532,7 @@
         <v>38.270000000000003</v>
       </c>
     </row>
-    <row r="450" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" t="s">
         <v>472</v>
       </c>
@@ -11487,7 +11558,7 @@
         <v>40.97</v>
       </c>
     </row>
-    <row r="451" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" t="s">
         <v>473</v>
       </c>
@@ -11513,7 +11584,7 @@
         <v>21.98</v>
       </c>
     </row>
-    <row r="452" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" t="s">
         <v>474</v>
       </c>
@@ -11539,7 +11610,7 @@
         <v>62.28</v>
       </c>
     </row>
-    <row r="453" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A453" t="s">
         <v>475</v>
       </c>
@@ -11555,8 +11626,14 @@
       <c r="E453" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="454" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H453">
+        <v>22.28</v>
+      </c>
+      <c r="I453">
+        <v>61.77</v>
+      </c>
+    </row>
+    <row r="454" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A454" t="s">
         <v>476</v>
       </c>
@@ -11572,8 +11649,14 @@
       <c r="E454" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="455" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H454">
+        <v>14.77</v>
+      </c>
+      <c r="I454">
+        <v>51.35</v>
+      </c>
+    </row>
+    <row r="455" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A455" t="s">
         <v>477</v>
       </c>
@@ -11589,8 +11672,14 @@
       <c r="E455" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="456" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H455">
+        <v>13.31</v>
+      </c>
+      <c r="I455">
+        <v>38.04</v>
+      </c>
+    </row>
+    <row r="456" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A456" t="s">
         <v>478</v>
       </c>
@@ -11606,8 +11695,17 @@
       <c r="E456" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="457" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H456">
+        <v>11.67</v>
+      </c>
+      <c r="I456">
+        <v>55.94</v>
+      </c>
+      <c r="J456" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="457" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A457" t="s">
         <v>479</v>
       </c>
@@ -11623,8 +11721,14 @@
       <c r="E457" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="458" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H457">
+        <v>13.51</v>
+      </c>
+      <c r="I457">
+        <v>55.18</v>
+      </c>
+    </row>
+    <row r="458" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" t="s">
         <v>480</v>
       </c>
@@ -11640,8 +11744,14 @@
       <c r="E458" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="459" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H458">
+        <v>7.29</v>
+      </c>
+      <c r="I458">
+        <v>30.39</v>
+      </c>
+    </row>
+    <row r="459" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" t="s">
         <v>481</v>
       </c>
@@ -11657,8 +11767,14 @@
       <c r="E459" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="460" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H459">
+        <v>7.25</v>
+      </c>
+      <c r="I459">
+        <v>21.68</v>
+      </c>
+    </row>
+    <row r="460" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" t="s">
         <v>482</v>
       </c>
@@ -11674,8 +11790,14 @@
       <c r="E460" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="461" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H460">
+        <v>19.29</v>
+      </c>
+      <c r="I460">
+        <v>54.55</v>
+      </c>
+    </row>
+    <row r="461" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" t="s">
         <v>483</v>
       </c>
@@ -11691,8 +11813,14 @@
       <c r="E461" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="462" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H461">
+        <v>6.47</v>
+      </c>
+      <c r="I461">
+        <v>20.78</v>
+      </c>
+    </row>
+    <row r="462" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
         <v>484</v>
       </c>
@@ -11708,8 +11836,14 @@
       <c r="E462" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="463" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H462">
+        <v>18.37</v>
+      </c>
+      <c r="I462">
+        <v>40.85</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" t="s">
         <v>485</v>
       </c>
@@ -11735,7 +11869,7 @@
         <v>26.77</v>
       </c>
     </row>
-    <row r="464" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
         <v>486</v>
       </c>
@@ -11839,7 +11973,7 @@
         <v>83.53</v>
       </c>
     </row>
-    <row r="468" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A468" t="s">
         <v>490</v>
       </c>
@@ -11855,8 +11989,14 @@
       <c r="E468" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="469" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H468">
+        <v>20.69</v>
+      </c>
+      <c r="I468">
+        <v>58.42</v>
+      </c>
+    </row>
+    <row r="469" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A469" t="s">
         <v>491</v>
       </c>
@@ -11872,8 +12012,14 @@
       <c r="E469" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="470" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H469">
+        <v>8.76</v>
+      </c>
+      <c r="I469">
+        <v>33.19</v>
+      </c>
+    </row>
+    <row r="470" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A470" t="s">
         <v>492</v>
       </c>
@@ -11889,8 +12035,14 @@
       <c r="E470" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="471" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H470">
+        <v>12.45</v>
+      </c>
+      <c r="I470">
+        <v>44.83</v>
+      </c>
+    </row>
+    <row r="471" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A471" t="s">
         <v>493</v>
       </c>
@@ -11906,8 +12058,14 @@
       <c r="E471" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="472" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H471">
+        <v>14.59</v>
+      </c>
+      <c r="I471">
+        <v>44.47</v>
+      </c>
+    </row>
+    <row r="472" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A472" t="s">
         <v>494</v>
       </c>
@@ -11922,6 +12080,12 @@
       </c>
       <c r="E472" t="s">
         <v>460</v>
+      </c>
+      <c r="H472">
+        <v>7.98</v>
+      </c>
+      <c r="I472">
+        <v>29.83</v>
       </c>
     </row>
     <row r="473" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -11940,6 +12104,12 @@
       <c r="E473" t="s">
         <v>460</v>
       </c>
+      <c r="H473">
+        <v>10.79</v>
+      </c>
+      <c r="I473">
+        <v>57.83</v>
+      </c>
     </row>
     <row r="474" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A474" t="s">
@@ -11957,6 +12127,12 @@
       <c r="E474" t="s">
         <v>460</v>
       </c>
+      <c r="H474">
+        <v>6.81</v>
+      </c>
+      <c r="I474">
+        <v>35.54</v>
+      </c>
     </row>
     <row r="475" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A475" t="s">
@@ -11974,6 +12150,12 @@
       <c r="E475" t="s">
         <v>460</v>
       </c>
+      <c r="H475">
+        <v>11.67</v>
+      </c>
+      <c r="I475">
+        <v>22.54</v>
+      </c>
     </row>
     <row r="476" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A476" t="s">
@@ -11991,6 +12173,12 @@
       <c r="E476" t="s">
         <v>460</v>
       </c>
+      <c r="H476">
+        <v>17.82</v>
+      </c>
+      <c r="I476">
+        <v>70.75</v>
+      </c>
     </row>
     <row r="477" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A477" t="s">
@@ -12008,6 +12196,12 @@
       <c r="E477" t="s">
         <v>460</v>
       </c>
+      <c r="H477">
+        <v>11.03</v>
+      </c>
+      <c r="I477">
+        <v>67.19</v>
+      </c>
     </row>
     <row r="478" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A478" t="s">
@@ -12142,7 +12336,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="483" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A483" t="s">
         <v>505</v>
       </c>
@@ -12158,8 +12352,14 @@
       <c r="E483" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="484" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H483">
+        <v>6.79</v>
+      </c>
+      <c r="I483">
+        <v>56.46</v>
+      </c>
+    </row>
+    <row r="484" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A484" t="s">
         <v>506</v>
       </c>
@@ -12175,8 +12375,14 @@
       <c r="E484" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="485" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H484">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I484">
+        <v>38.25</v>
+      </c>
+    </row>
+    <row r="485" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A485" t="s">
         <v>507</v>
       </c>
@@ -12192,8 +12398,14 @@
       <c r="E485" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="486" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H485">
+        <v>4.97</v>
+      </c>
+      <c r="I485">
+        <v>15.12</v>
+      </c>
+    </row>
+    <row r="486" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A486" t="s">
         <v>508</v>
       </c>
@@ -12209,8 +12421,14 @@
       <c r="E486" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="487" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H486">
+        <v>6.82</v>
+      </c>
+      <c r="I486">
+        <v>24.19</v>
+      </c>
+    </row>
+    <row r="487" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A487" t="s">
         <v>509</v>
       </c>
@@ -12225,6 +12443,12 @@
       </c>
       <c r="E487" t="s">
         <v>460</v>
+      </c>
+      <c r="H487">
+        <v>9.93</v>
+      </c>
+      <c r="I487">
+        <v>43.38</v>
       </c>
     </row>
     <row r="488" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -12243,6 +12467,12 @@
       <c r="E488" t="s">
         <v>460</v>
       </c>
+      <c r="H488">
+        <v>8.06</v>
+      </c>
+      <c r="I488">
+        <v>39.24</v>
+      </c>
     </row>
     <row r="489" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A489" t="s">
@@ -12260,6 +12490,12 @@
       <c r="E489" t="s">
         <v>460</v>
       </c>
+      <c r="H489">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I489">
+        <v>39.14</v>
+      </c>
     </row>
     <row r="490" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A490" t="s">
@@ -12277,6 +12513,12 @@
       <c r="E490" t="s">
         <v>460</v>
       </c>
+      <c r="H490">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="I490">
+        <v>55.41</v>
+      </c>
     </row>
     <row r="491" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A491" t="s">
@@ -12294,6 +12536,12 @@
       <c r="E491" t="s">
         <v>460</v>
       </c>
+      <c r="H491">
+        <v>12.5</v>
+      </c>
+      <c r="I491">
+        <v>35.01</v>
+      </c>
     </row>
     <row r="492" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A492" t="s">
@@ -12311,6 +12559,12 @@
       <c r="E492" t="s">
         <v>460</v>
       </c>
+      <c r="H492">
+        <v>8.4700000000000006</v>
+      </c>
+      <c r="I492">
+        <v>28.45</v>
+      </c>
     </row>
     <row r="493" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A493" t="s">
@@ -12442,7 +12696,7 @@
         <v>48.38</v>
       </c>
     </row>
-    <row r="498" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A498" t="s">
         <v>520</v>
       </c>
@@ -12458,8 +12712,14 @@
       <c r="E498" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="499" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H498">
+        <v>11.38</v>
+      </c>
+      <c r="I498">
+        <v>61.14</v>
+      </c>
+    </row>
+    <row r="499" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A499" t="s">
         <v>521</v>
       </c>
@@ -12475,8 +12735,14 @@
       <c r="E499" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="500" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H499">
+        <v>12.19</v>
+      </c>
+      <c r="I499">
+        <v>53.43</v>
+      </c>
+    </row>
+    <row r="500" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A500" t="s">
         <v>522</v>
       </c>
@@ -12492,8 +12758,14 @@
       <c r="E500" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="501" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H500">
+        <v>7.53</v>
+      </c>
+      <c r="I500">
+        <v>38.39</v>
+      </c>
+    </row>
+    <row r="501" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A501" t="s">
         <v>523</v>
       </c>
@@ -12509,8 +12781,14 @@
       <c r="E501" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="502" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H501">
+        <v>12.29</v>
+      </c>
+      <c r="I501">
+        <v>55.25</v>
+      </c>
+    </row>
+    <row r="502" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A502" t="s">
         <v>524</v>
       </c>
@@ -12525,6 +12803,12 @@
       </c>
       <c r="E502" t="s">
         <v>460</v>
+      </c>
+      <c r="H502">
+        <v>17.41</v>
+      </c>
+      <c r="I502">
+        <v>38.53</v>
       </c>
     </row>
     <row r="503" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -12543,6 +12827,15 @@
       <c r="E503" t="s">
         <v>460</v>
       </c>
+      <c r="F503" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="H503" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="I503" s="2" t="s">
+        <v>645</v>
+      </c>
     </row>
     <row r="504" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504" t="s">
@@ -12560,6 +12853,12 @@
       <c r="E504" t="s">
         <v>460</v>
       </c>
+      <c r="H504">
+        <v>4.2</v>
+      </c>
+      <c r="I504">
+        <v>11.66</v>
+      </c>
     </row>
     <row r="505" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A505" t="s">
@@ -12577,6 +12876,12 @@
       <c r="E505" t="s">
         <v>460</v>
       </c>
+      <c r="H505">
+        <v>7.83</v>
+      </c>
+      <c r="I505">
+        <v>56.11</v>
+      </c>
     </row>
     <row r="506" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A506" t="s">
@@ -12594,6 +12899,12 @@
       <c r="E506" t="s">
         <v>460</v>
       </c>
+      <c r="H506">
+        <v>10.039999999999999</v>
+      </c>
+      <c r="I506">
+        <v>54.09</v>
+      </c>
     </row>
     <row r="507" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A507" t="s">
@@ -12611,6 +12922,12 @@
       <c r="E507" t="s">
         <v>460</v>
       </c>
+      <c r="H507">
+        <v>6.14</v>
+      </c>
+      <c r="I507">
+        <v>22.19</v>
+      </c>
     </row>
     <row r="508" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A508" t="s">
@@ -12742,7 +13059,7 @@
         <v>26.14</v>
       </c>
     </row>
-    <row r="513" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A513" t="s">
         <v>535</v>
       </c>
@@ -12758,8 +13075,14 @@
       <c r="E513" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="514" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H513">
+        <v>10.77</v>
+      </c>
+      <c r="I513">
+        <v>47.33</v>
+      </c>
+    </row>
+    <row r="514" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
         <v>536</v>
       </c>
@@ -12775,8 +13098,14 @@
       <c r="E514" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="515" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H514">
+        <v>6.13</v>
+      </c>
+      <c r="I514">
+        <v>26.89</v>
+      </c>
+    </row>
+    <row r="515" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
         <v>537</v>
       </c>
@@ -12792,8 +13121,14 @@
       <c r="E515" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="516" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H515">
+        <v>4.49</v>
+      </c>
+      <c r="I515">
+        <v>17.11</v>
+      </c>
+    </row>
+    <row r="516" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
         <v>538</v>
       </c>
@@ -12809,8 +13144,14 @@
       <c r="E516" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="517" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H516">
+        <v>6.15</v>
+      </c>
+      <c r="I516">
+        <v>25.55</v>
+      </c>
+    </row>
+    <row r="517" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
         <v>539</v>
       </c>
@@ -12825,6 +13166,12 @@
       </c>
       <c r="E517" t="s">
         <v>460</v>
+      </c>
+      <c r="H517">
+        <v>11.15</v>
+      </c>
+      <c r="I517">
+        <v>49.87</v>
       </c>
     </row>
     <row r="518" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -12843,6 +13190,12 @@
       <c r="E518" t="s">
         <v>460</v>
       </c>
+      <c r="H518">
+        <v>6.94</v>
+      </c>
+      <c r="I518">
+        <v>35.89</v>
+      </c>
     </row>
     <row r="519" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
@@ -12860,6 +13213,12 @@
       <c r="E519" t="s">
         <v>460</v>
       </c>
+      <c r="H519">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="I519">
+        <v>38.47</v>
+      </c>
     </row>
     <row r="520" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A520" t="s">
@@ -12877,6 +13236,12 @@
       <c r="E520" t="s">
         <v>460</v>
       </c>
+      <c r="H520">
+        <v>13.49</v>
+      </c>
+      <c r="I520">
+        <v>38.25</v>
+      </c>
     </row>
     <row r="521" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A521" t="s">
@@ -12894,6 +13259,12 @@
       <c r="E521" t="s">
         <v>460</v>
       </c>
+      <c r="H521">
+        <v>15.93</v>
+      </c>
+      <c r="I521">
+        <v>61.28</v>
+      </c>
     </row>
     <row r="522" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
@@ -12910,6 +13281,12 @@
       </c>
       <c r="E522" t="s">
         <v>460</v>
+      </c>
+      <c r="H522">
+        <v>5.4</v>
+      </c>
+      <c r="I522">
+        <v>27.75</v>
       </c>
     </row>
     <row r="523" spans="1:9" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
biomass for all 3 blocs Segi
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/biomass.xlsx
+++ b/data/treeMeasurements/biomass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41F6458-F5C8-BE4E-90EA-AA525B106782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D515E362-0247-E146-AF39-00D85BABF98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -2029,9 +2029,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2107,7 +2108,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>527</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2195,14 +2196,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I617" totalsRowShown="0">
   <autoFilter ref="A1:I617" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="pinus_strobus"/>
+        <filter val="sequoiadendron_giganteum"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2501,9 +2497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J617"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I247" sqref="I247"/>
+    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I557" sqref="I557"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6502,7 +6498,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>203</v>
       </c>
@@ -6525,7 +6521,7 @@
         <v>20.94</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>204</v>
       </c>
@@ -6548,7 +6544,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>205</v>
       </c>
@@ -6571,7 +6567,7 @@
         <v>44.4</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>206</v>
       </c>
@@ -6594,7 +6590,7 @@
         <v>50.91</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>207</v>
       </c>
@@ -6817,7 +6813,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>218</v>
       </c>
@@ -6840,7 +6836,7 @@
         <v>34.520000000000003</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>219</v>
       </c>
@@ -6863,7 +6859,7 @@
         <v>90.64</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>220</v>
       </c>
@@ -6886,7 +6882,7 @@
         <v>30.06</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>221</v>
       </c>
@@ -6909,7 +6905,7 @@
         <v>70.38</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>222</v>
       </c>
@@ -7132,7 +7128,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>233</v>
       </c>
@@ -7155,7 +7151,7 @@
         <v>19.559999999999999</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>234</v>
       </c>
@@ -7178,7 +7174,7 @@
         <v>73.66</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>235</v>
       </c>
@@ -7201,7 +7197,7 @@
         <v>47.45</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>236</v>
       </c>
@@ -7224,7 +7220,7 @@
         <v>39.21</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>237</v>
       </c>
@@ -7447,7 +7443,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>248</v>
       </c>
@@ -7470,7 +7466,7 @@
         <v>69.41</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>249</v>
       </c>
@@ -7493,7 +7489,7 @@
         <v>35.47</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>250</v>
       </c>
@@ -7516,7 +7512,7 @@
         <v>50.72</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>251</v>
       </c>
@@ -7539,7 +7535,7 @@
         <v>47.92</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>252</v>
       </c>
@@ -7762,7 +7758,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>263</v>
       </c>
@@ -7785,7 +7781,7 @@
         <v>40.76</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>264</v>
       </c>
@@ -7808,7 +7804,7 @@
         <v>45.4</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>265</v>
       </c>
@@ -7831,7 +7827,7 @@
         <v>59.33</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>266</v>
       </c>
@@ -7854,7 +7850,7 @@
         <v>43.07</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>267</v>
       </c>
@@ -8077,7 +8073,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>278</v>
       </c>
@@ -8100,7 +8096,7 @@
         <v>49.89</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>279</v>
       </c>
@@ -8123,7 +8119,7 @@
         <v>33.119999999999997</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>280</v>
       </c>
@@ -8149,7 +8145,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>281</v>
       </c>
@@ -8172,7 +8168,7 @@
         <v>47.58</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>282</v>
       </c>
@@ -13784,7 +13780,7 @@
         <v>38.96</v>
       </c>
     </row>
-    <row r="528" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>550</v>
       </c>
@@ -13801,7 +13797,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="529" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>553</v>
       </c>
@@ -13817,8 +13813,14 @@
       <c r="E529" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="530" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H529">
+        <v>35.380000000000003</v>
+      </c>
+      <c r="I529">
+        <v>47.81</v>
+      </c>
+    </row>
+    <row r="530" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>554</v>
       </c>
@@ -13834,8 +13836,10 @@
       <c r="E530" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="531" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H530" s="2"/>
+      <c r="I530" s="2"/>
+    </row>
+    <row r="531" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>555</v>
       </c>
@@ -13851,8 +13855,14 @@
       <c r="E531" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="532" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H531">
+        <v>15.5</v>
+      </c>
+      <c r="I531">
+        <v>18.84</v>
+      </c>
+    </row>
+    <row r="532" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>556</v>
       </c>
@@ -13868,8 +13878,14 @@
       <c r="E532" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="533" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H532">
+        <v>15.29</v>
+      </c>
+      <c r="I532">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>557</v>
       </c>
@@ -13885,8 +13901,14 @@
       <c r="E533" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="534" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H533">
+        <v>30.8</v>
+      </c>
+      <c r="I533">
+        <v>46.47</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>558</v>
       </c>
@@ -13902,8 +13924,14 @@
       <c r="E534" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="535" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H534">
+        <v>33.659999999999997</v>
+      </c>
+      <c r="I534">
+        <v>58.75</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>559</v>
       </c>
@@ -13919,8 +13947,14 @@
       <c r="E535" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="536" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H535">
+        <v>22.08</v>
+      </c>
+      <c r="I535">
+        <v>40.49</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>560</v>
       </c>
@@ -13936,8 +13970,14 @@
       <c r="E536" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="537" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H536">
+        <v>19.739999999999998</v>
+      </c>
+      <c r="I536">
+        <v>22.01</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>561</v>
       </c>
@@ -13953,8 +13993,14 @@
       <c r="E537" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="538" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H537">
+        <v>26.22</v>
+      </c>
+      <c r="I537">
+        <v>38.18</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>562</v>
       </c>
@@ -13971,7 +14017,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="539" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>563</v>
       </c>
@@ -13987,8 +14033,14 @@
       <c r="E539" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="540" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H539">
+        <v>14.05</v>
+      </c>
+      <c r="I539">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>564</v>
       </c>
@@ -14005,7 +14057,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="541" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>565</v>
       </c>
@@ -14021,8 +14073,14 @@
       <c r="E541" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="542" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H541">
+        <v>11.88</v>
+      </c>
+      <c r="I541">
+        <v>11.61</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>566</v>
       </c>
@@ -14038,8 +14096,14 @@
       <c r="E542" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="543" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H542">
+        <v>24.99</v>
+      </c>
+      <c r="I542">
+        <v>25.56</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>567</v>
       </c>
@@ -14056,7 +14120,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="544" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>568</v>
       </c>
@@ -14072,8 +14136,14 @@
       <c r="E544" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="545" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H544">
+        <v>19.54</v>
+      </c>
+      <c r="I544">
+        <v>24.46</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
         <v>569</v>
       </c>
@@ -14089,8 +14159,14 @@
       <c r="E545" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="546" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H545">
+        <v>35.56</v>
+      </c>
+      <c r="I545">
+        <v>44.88</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>570</v>
       </c>
@@ -14106,8 +14182,14 @@
       <c r="E546" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="547" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H546">
+        <v>16.82</v>
+      </c>
+      <c r="I546">
+        <v>23.17</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
         <v>571</v>
       </c>
@@ -14123,8 +14205,14 @@
       <c r="E547" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="548" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H547">
+        <v>29.01</v>
+      </c>
+      <c r="I547">
+        <v>39.979999999999997</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>572</v>
       </c>
@@ -14140,8 +14228,14 @@
       <c r="E548" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="549" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H548">
+        <v>17.25</v>
+      </c>
+      <c r="I548">
+        <v>27.39</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
         <v>573</v>
       </c>
@@ -14157,8 +14251,14 @@
       <c r="E549" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="550" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H549">
+        <v>29.06</v>
+      </c>
+      <c r="I549">
+        <v>64.31</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>574</v>
       </c>
@@ -14174,8 +14274,14 @@
       <c r="E550" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="551" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H550">
+        <v>33.78</v>
+      </c>
+      <c r="I550">
+        <v>63.08</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
         <v>575</v>
       </c>
@@ -14191,8 +14297,14 @@
       <c r="E551" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="552" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H551">
+        <v>15.37</v>
+      </c>
+      <c r="I551">
+        <v>14.76</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>576</v>
       </c>
@@ -14209,7 +14321,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="553" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
         <v>577</v>
       </c>
@@ -14225,8 +14337,14 @@
       <c r="E553" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="554" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H553">
+        <v>25.2</v>
+      </c>
+      <c r="I553">
+        <v>36.450000000000003</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>578</v>
       </c>
@@ -14242,8 +14360,14 @@
       <c r="E554" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="555" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H554">
+        <v>30.79</v>
+      </c>
+      <c r="I554">
+        <v>45.38</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
         <v>579</v>
       </c>
@@ -14259,8 +14383,14 @@
       <c r="E555" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="556" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H555">
+        <v>30.6</v>
+      </c>
+      <c r="I555">
+        <v>52.68</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>580</v>
       </c>
@@ -14276,8 +14406,14 @@
       <c r="E556" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="557" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H556">
+        <v>30.11</v>
+      </c>
+      <c r="I556">
+        <v>38.04</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
         <v>581</v>
       </c>
@@ -14294,7 +14430,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="558" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>582</v>
       </c>
@@ -14310,8 +14446,14 @@
       <c r="E558" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="559" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H558">
+        <v>26.79</v>
+      </c>
+      <c r="I558">
+        <v>34.21</v>
+      </c>
+    </row>
+    <row r="559" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>583</v>
       </c>
@@ -14328,8 +14470,14 @@
         <v>552</v>
       </c>
       <c r="F559" s="1"/>
-    </row>
-    <row r="560" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H559">
+        <v>35.15</v>
+      </c>
+      <c r="I559">
+        <v>50.05</v>
+      </c>
+    </row>
+    <row r="560" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
         <v>584</v>
       </c>
@@ -14346,7 +14494,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="561" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>585</v>
       </c>
@@ -14363,7 +14511,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="562" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>586</v>
       </c>
@@ -14380,7 +14528,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="563" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>587</v>
       </c>
@@ -14396,8 +14544,14 @@
       <c r="E563" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="564" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H563">
+        <v>27.72</v>
+      </c>
+      <c r="I563">
+        <v>48.09</v>
+      </c>
+    </row>
+    <row r="564" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>588</v>
       </c>
@@ -14414,7 +14568,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="565" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>589</v>
       </c>
@@ -14430,8 +14584,14 @@
       <c r="E565" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="566" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H565">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="I565">
+        <v>49.77</v>
+      </c>
+    </row>
+    <row r="566" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>590</v>
       </c>
@@ -14447,8 +14607,14 @@
       <c r="E566" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="567" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H566">
+        <v>24.25</v>
+      </c>
+      <c r="I566">
+        <v>32.090000000000003</v>
+      </c>
+    </row>
+    <row r="567" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>591</v>
       </c>
@@ -14464,8 +14630,14 @@
       <c r="E567" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="568" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H567">
+        <v>25.92</v>
+      </c>
+      <c r="I567">
+        <v>39.06</v>
+      </c>
+    </row>
+    <row r="568" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>592</v>
       </c>
@@ -14482,8 +14654,14 @@
         <v>552</v>
       </c>
       <c r="F568" s="1"/>
-    </row>
-    <row r="569" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H568">
+        <v>33.619999999999997</v>
+      </c>
+      <c r="I568">
+        <v>51.09</v>
+      </c>
+    </row>
+    <row r="569" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>593</v>
       </c>
@@ -14500,7 +14678,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="570" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>594</v>
       </c>
@@ -14516,8 +14694,14 @@
       <c r="E570" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="571" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H570">
+        <v>23.24</v>
+      </c>
+      <c r="I570">
+        <v>31.86</v>
+      </c>
+    </row>
+    <row r="571" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>595</v>
       </c>
@@ -14533,8 +14717,14 @@
       <c r="E571" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="572" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H571">
+        <v>41.91</v>
+      </c>
+      <c r="I571">
+        <v>59.87</v>
+      </c>
+    </row>
+    <row r="572" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
         <v>596</v>
       </c>
@@ -14550,8 +14740,14 @@
       <c r="E572" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="573" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H572">
+        <v>41.19</v>
+      </c>
+      <c r="I572">
+        <v>65.760000000000005</v>
+      </c>
+    </row>
+    <row r="573" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
         <v>597</v>
       </c>
@@ -14567,8 +14763,14 @@
       <c r="E573" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="574" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H573">
+        <v>21.14</v>
+      </c>
+      <c r="I573">
+        <v>25.87</v>
+      </c>
+    </row>
+    <row r="574" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>598</v>
       </c>
@@ -14585,7 +14787,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="575" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
         <v>599</v>
       </c>
@@ -14602,7 +14804,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="576" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
         <v>600</v>
       </c>
@@ -14619,7 +14821,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="577" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
         <v>601</v>
       </c>
@@ -14635,8 +14837,14 @@
       <c r="E577" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="578" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H577">
+        <v>4.74</v>
+      </c>
+      <c r="I577">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="578" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
         <v>602</v>
       </c>
@@ -14652,8 +14860,14 @@
       <c r="E578" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="579" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H578">
+        <v>52</v>
+      </c>
+      <c r="I578">
+        <v>102.04</v>
+      </c>
+    </row>
+    <row r="579" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
         <v>603</v>
       </c>
@@ -14669,8 +14883,14 @@
       <c r="E579" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="580" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H579">
+        <v>35.19</v>
+      </c>
+      <c r="I579">
+        <v>60.99</v>
+      </c>
+    </row>
+    <row r="580" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
         <v>604</v>
       </c>
@@ -14686,8 +14906,14 @@
       <c r="E580" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="581" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H580">
+        <v>35.83</v>
+      </c>
+      <c r="I580">
+        <v>54.2</v>
+      </c>
+    </row>
+    <row r="581" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
         <v>605</v>
       </c>
@@ -14703,8 +14929,14 @@
       <c r="E581" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="582" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H581">
+        <v>28.44</v>
+      </c>
+      <c r="I581">
+        <v>49.65</v>
+      </c>
+    </row>
+    <row r="582" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
         <v>606</v>
       </c>
@@ -14720,8 +14952,14 @@
       <c r="E582" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="583" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H582">
+        <v>5.77</v>
+      </c>
+      <c r="I582">
+        <v>3.29</v>
+      </c>
+    </row>
+    <row r="583" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A583" t="s">
         <v>607</v>
       </c>
@@ -14737,8 +14975,14 @@
       <c r="E583" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="584" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H583">
+        <v>15.73</v>
+      </c>
+      <c r="I583">
+        <v>23.04</v>
+      </c>
+    </row>
+    <row r="584" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
         <v>608</v>
       </c>
@@ -14754,8 +14998,14 @@
       <c r="E584" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="585" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H584">
+        <v>28.36</v>
+      </c>
+      <c r="I584">
+        <v>29.88</v>
+      </c>
+    </row>
+    <row r="585" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
         <v>609</v>
       </c>
@@ -14771,8 +15021,14 @@
       <c r="E585" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="586" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H585">
+        <v>38</v>
+      </c>
+      <c r="I585">
+        <v>54.6</v>
+      </c>
+    </row>
+    <row r="586" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
         <v>610</v>
       </c>
@@ -14788,8 +15044,14 @@
       <c r="E586" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="587" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H586">
+        <v>27.58</v>
+      </c>
+      <c r="I586">
+        <v>36.08</v>
+      </c>
+    </row>
+    <row r="587" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
         <v>611</v>
       </c>
@@ -14806,7 +15068,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="588" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
         <v>612</v>
       </c>
@@ -14822,8 +15084,14 @@
       <c r="E588" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="589" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H588">
+        <v>32.950000000000003</v>
+      </c>
+      <c r="I588">
+        <v>42.14</v>
+      </c>
+    </row>
+    <row r="589" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
         <v>613</v>
       </c>
@@ -14840,7 +15108,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="590" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
         <v>614</v>
       </c>
@@ -14857,7 +15125,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="591" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
         <v>615</v>
       </c>
@@ -14874,7 +15142,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="592" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
         <v>616</v>
       </c>
@@ -14890,8 +15158,14 @@
       <c r="E592" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="593" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H592">
+        <v>14.27</v>
+      </c>
+      <c r="I592">
+        <v>14.62</v>
+      </c>
+    </row>
+    <row r="593" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
         <v>617</v>
       </c>
@@ -14907,8 +15181,14 @@
       <c r="E593" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="594" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H593" s="2">
+        <v>24.84</v>
+      </c>
+      <c r="I593" s="2">
+        <v>40.42</v>
+      </c>
+    </row>
+    <row r="594" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
         <v>618</v>
       </c>
@@ -14924,8 +15204,14 @@
       <c r="E594" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="595" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H594">
+        <v>36.049999999999997</v>
+      </c>
+      <c r="I594">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="595" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>619</v>
       </c>
@@ -14942,7 +15228,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="596" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
         <v>620</v>
       </c>
@@ -14958,8 +15244,14 @@
       <c r="E596" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="597" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H596">
+        <v>18</v>
+      </c>
+      <c r="I596">
+        <v>25.61</v>
+      </c>
+    </row>
+    <row r="597" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>621</v>
       </c>
@@ -14976,7 +15268,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="598" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
         <v>622</v>
       </c>
@@ -14993,7 +15285,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="599" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>623</v>
       </c>
@@ -15009,8 +15301,14 @@
       <c r="E599" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="600" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H599">
+        <v>23.6</v>
+      </c>
+      <c r="I599">
+        <v>30.13</v>
+      </c>
+    </row>
+    <row r="600" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
         <v>624</v>
       </c>
@@ -15026,8 +15324,14 @@
       <c r="E600" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="601" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H600">
+        <v>31.43</v>
+      </c>
+      <c r="I600">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="601" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
         <v>625</v>
       </c>
@@ -15043,8 +15347,14 @@
       <c r="E601" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="602" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H601">
+        <v>14.47</v>
+      </c>
+      <c r="I601">
+        <v>15.12</v>
+      </c>
+    </row>
+    <row r="602" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
         <v>626</v>
       </c>
@@ -15060,8 +15370,14 @@
       <c r="E602" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="603" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H602">
+        <v>39.03</v>
+      </c>
+      <c r="I602">
+        <v>46.17</v>
+      </c>
+    </row>
+    <row r="603" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
         <v>627</v>
       </c>
@@ -15077,8 +15393,14 @@
       <c r="E603" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="604" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H603">
+        <v>24.38</v>
+      </c>
+      <c r="I603">
+        <v>36.78</v>
+      </c>
+    </row>
+    <row r="604" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
         <v>628</v>
       </c>
@@ -15094,8 +15416,14 @@
       <c r="E604" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="605" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H604">
+        <v>7.74</v>
+      </c>
+      <c r="I604">
+        <v>6.78</v>
+      </c>
+    </row>
+    <row r="605" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
         <v>629</v>
       </c>
@@ -15111,8 +15439,14 @@
       <c r="E605" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="606" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H605">
+        <v>27.09</v>
+      </c>
+      <c r="I605">
+        <v>47.97</v>
+      </c>
+    </row>
+    <row r="606" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
         <v>630</v>
       </c>
@@ -15128,8 +15462,9 @@
       <c r="E606" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="607" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H606" s="2"/>
+    </row>
+    <row r="607" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
         <v>631</v>
       </c>
@@ -15145,8 +15480,14 @@
       <c r="E607" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="608" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H607">
+        <v>18.71</v>
+      </c>
+      <c r="I607">
+        <v>29.54</v>
+      </c>
+    </row>
+    <row r="608" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
         <v>632</v>
       </c>
@@ -15162,8 +15503,14 @@
       <c r="E608" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="609" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H608">
+        <v>31.13</v>
+      </c>
+      <c r="I608">
+        <v>51.46</v>
+      </c>
+    </row>
+    <row r="609" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
         <v>633</v>
       </c>
@@ -15179,8 +15526,14 @@
       <c r="E609" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="610" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H609">
+        <v>17.68</v>
+      </c>
+      <c r="I609">
+        <v>28.47</v>
+      </c>
+    </row>
+    <row r="610" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
         <v>634</v>
       </c>
@@ -15196,8 +15549,14 @@
       <c r="E610" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="611" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H610">
+        <v>32.22</v>
+      </c>
+      <c r="I610">
+        <v>41.69</v>
+      </c>
+    </row>
+    <row r="611" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
         <v>635</v>
       </c>
@@ -15213,8 +15572,14 @@
       <c r="E611" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="612" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H611">
+        <v>33.020000000000003</v>
+      </c>
+      <c r="I611">
+        <v>49.01</v>
+      </c>
+    </row>
+    <row r="612" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
         <v>636</v>
       </c>
@@ -15230,8 +15595,14 @@
       <c r="E612" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="613" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H612">
+        <v>25.97</v>
+      </c>
+      <c r="I612">
+        <v>38.869999999999997</v>
+      </c>
+    </row>
+    <row r="613" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>637</v>
       </c>
@@ -15247,8 +15618,14 @@
       <c r="E613" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="614" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H613">
+        <v>26.24</v>
+      </c>
+      <c r="I613">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="614" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
         <v>638</v>
       </c>
@@ -15264,8 +15641,14 @@
       <c r="E614" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="615" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H614">
+        <v>25.97</v>
+      </c>
+      <c r="I614">
+        <v>28.78</v>
+      </c>
+    </row>
+    <row r="615" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
         <v>639</v>
       </c>
@@ -15281,8 +15664,14 @@
       <c r="E615" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="616" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H615">
+        <v>37.270000000000003</v>
+      </c>
+      <c r="I615">
+        <v>44.41</v>
+      </c>
+    </row>
+    <row r="616" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>640</v>
       </c>
@@ -15298,8 +15687,14 @@
       <c r="E616" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="617" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H616">
+        <v>27.48</v>
+      </c>
+      <c r="I616">
+        <v>29.08</v>
+      </c>
+    </row>
+    <row r="617" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
         <v>641</v>
       </c>
@@ -15314,6 +15709,12 @@
       </c>
       <c r="E617" t="s">
         <v>552</v>
+      </c>
+      <c r="H617">
+        <v>23.3</v>
+      </c>
+      <c r="I617">
+        <v>29.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last pine bloc and bepa all bloc weighted!
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/biomass.xlsx
+++ b/data/treeMeasurements/biomass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D515E362-0247-E146-AF39-00D85BABF98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8AC9CC-A322-3044-8819-A04EE48884BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-2480" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -1989,7 +1989,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2005,6 +2005,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -2029,10 +2036,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2108,7 +2116,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>527</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2198,7 +2206,7 @@
   <autoFilter ref="A1:I617" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="4">
       <filters>
-        <filter val="sequoiadendron_giganteum"/>
+        <filter val="betula_papyrifera"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2497,9 +2505,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J617"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I557" sqref="I557"/>
+    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H155" sqref="H155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2513,7 +2521,7 @@
     <col min="9" max="10" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2541,8 +2549,9 @@
       <c r="I1" s="1" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2568,7 +2577,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2594,7 +2603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2620,7 +2629,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2646,7 +2655,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2672,7 +2681,7 @@
         <v>23.8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>23.18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2724,7 +2733,7 @@
         <v>13.67</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -2750,7 +2759,7 @@
         <v>16.239999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -2776,7 +2785,7 @@
         <v>18.260000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2802,7 +2811,7 @@
         <v>14.04</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -2828,7 +2837,7 @@
         <v>8.67</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -2854,7 +2863,7 @@
         <v>4.1399999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2880,7 +2889,7 @@
         <v>8.39</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>9.85</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -4882,7 +4891,7 @@
         <v>17.54</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -4898,8 +4907,18 @@
       <c r="E92" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G92">
+        <v>346</v>
+      </c>
+      <c r="H92">
+        <v>13.02</v>
+      </c>
+      <c r="I92">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J92</f>
+        <v>19.12</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -4915,8 +4934,18 @@
       <c r="E93" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G93">
+        <v>346</v>
+      </c>
+      <c r="H93">
+        <v>13.35</v>
+      </c>
+      <c r="I93">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J93</f>
+        <v>12.95</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -4932,8 +4961,18 @@
       <c r="E94" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G94">
+        <v>346</v>
+      </c>
+      <c r="H94">
+        <v>9.57</v>
+      </c>
+      <c r="I94">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J94</f>
+        <v>16.260000000000002</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -4949,8 +4988,18 @@
       <c r="E95" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G95">
+        <v>346</v>
+      </c>
+      <c r="H95">
+        <v>27.74</v>
+      </c>
+      <c r="I95">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J95</f>
+        <v>25.59</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -4966,8 +5015,18 @@
       <c r="E96" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G96">
+        <v>346</v>
+      </c>
+      <c r="H96">
+        <v>10.95</v>
+      </c>
+      <c r="I96">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J96</f>
+        <v>17.649999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -4983,8 +5042,18 @@
       <c r="E97" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G97">
+        <v>346</v>
+      </c>
+      <c r="H97">
+        <v>26.12</v>
+      </c>
+      <c r="I97">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J97</f>
+        <v>29.51</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -5000,8 +5069,18 @@
       <c r="E98" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G98">
+        <v>346</v>
+      </c>
+      <c r="H98">
+        <v>18.190000000000001</v>
+      </c>
+      <c r="I98">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J98</f>
+        <v>26.55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -5017,8 +5096,18 @@
       <c r="E99" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G99">
+        <v>346</v>
+      </c>
+      <c r="H99">
+        <v>43.15</v>
+      </c>
+      <c r="I99">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J99</f>
+        <v>38.93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -5034,8 +5123,18 @@
       <c r="E100" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G100">
+        <v>346</v>
+      </c>
+      <c r="H100">
+        <v>23.12</v>
+      </c>
+      <c r="I100">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J100</f>
+        <v>32.869999999999997</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -5051,8 +5150,18 @@
       <c r="E101" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G101">
+        <v>346</v>
+      </c>
+      <c r="H101">
+        <v>18.78</v>
+      </c>
+      <c r="I101">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J101</f>
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -5068,8 +5177,18 @@
       <c r="E102" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G102">
+        <v>346</v>
+      </c>
+      <c r="H102">
+        <v>13.61</v>
+      </c>
+      <c r="I102">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J102</f>
+        <v>20.329999999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -5085,8 +5204,18 @@
       <c r="E103" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G103">
+        <v>346</v>
+      </c>
+      <c r="H103">
+        <v>17.71</v>
+      </c>
+      <c r="I103">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J103</f>
+        <v>12.17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -5102,8 +5231,18 @@
       <c r="E104" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G104">
+        <v>346</v>
+      </c>
+      <c r="H104">
+        <v>27.25</v>
+      </c>
+      <c r="I104">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J104</f>
+        <v>42.11</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -5119,8 +5258,18 @@
       <c r="E105" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G105">
+        <v>346</v>
+      </c>
+      <c r="H105">
+        <v>11.23</v>
+      </c>
+      <c r="I105">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J105</f>
+        <v>17.18</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -5137,8 +5286,18 @@
         <v>106</v>
       </c>
       <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G106">
+        <v>346</v>
+      </c>
+      <c r="H106">
+        <v>17.43</v>
+      </c>
+      <c r="I106">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J106</f>
+        <v>17.149999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>121</v>
       </c>
@@ -5154,8 +5313,18 @@
       <c r="E107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G107">
+        <v>346</v>
+      </c>
+      <c r="H107">
+        <v>35</v>
+      </c>
+      <c r="I107">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J107</f>
+        <v>38.83</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -5171,8 +5340,18 @@
       <c r="E108" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G108">
+        <v>346</v>
+      </c>
+      <c r="H108">
+        <v>18.73</v>
+      </c>
+      <c r="I108">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J108</f>
+        <v>14.95</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -5188,8 +5367,18 @@
       <c r="E109" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G109">
+        <v>346</v>
+      </c>
+      <c r="H109">
+        <v>16.66</v>
+      </c>
+      <c r="I109">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J109</f>
+        <v>17.559999999999999</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>124</v>
       </c>
@@ -5205,8 +5394,18 @@
       <c r="E110" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G110">
+        <v>346</v>
+      </c>
+      <c r="H110">
+        <v>16.36</v>
+      </c>
+      <c r="I110">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J110</f>
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>125</v>
       </c>
@@ -5222,8 +5421,18 @@
       <c r="E111" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G111">
+        <v>346</v>
+      </c>
+      <c r="H111">
+        <v>44.9</v>
+      </c>
+      <c r="I111">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J111</f>
+        <v>46.09</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -5239,8 +5448,18 @@
       <c r="E112" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G112">
+        <v>346</v>
+      </c>
+      <c r="H112">
+        <v>26.56</v>
+      </c>
+      <c r="I112">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J112</f>
+        <v>38.270000000000003</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -5256,8 +5475,18 @@
       <c r="E113" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G113">
+        <v>346</v>
+      </c>
+      <c r="H113">
+        <v>13.74</v>
+      </c>
+      <c r="I113">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J113</f>
+        <v>13.45</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -5273,8 +5502,18 @@
       <c r="E114" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G114">
+        <v>346</v>
+      </c>
+      <c r="H114">
+        <v>23.98</v>
+      </c>
+      <c r="I114">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J114</f>
+        <v>33.840000000000003</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -5290,8 +5529,18 @@
       <c r="E115" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G115">
+        <v>346</v>
+      </c>
+      <c r="H115">
+        <v>41.04</v>
+      </c>
+      <c r="I115">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J115</f>
+        <v>39.4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -5307,8 +5556,18 @@
       <c r="E116" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G116">
+        <v>346</v>
+      </c>
+      <c r="H116">
+        <v>8.86</v>
+      </c>
+      <c r="I116">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J116</f>
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -5324,8 +5583,18 @@
       <c r="E117" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G117">
+        <v>346</v>
+      </c>
+      <c r="H117" s="2">
+        <v>24.57</v>
+      </c>
+      <c r="I117">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J117</f>
+        <v>27.72</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>132</v>
       </c>
@@ -5341,8 +5610,18 @@
       <c r="E118" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G118">
+        <v>346</v>
+      </c>
+      <c r="H118">
+        <v>12.46</v>
+      </c>
+      <c r="I118">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J118</f>
+        <v>14.02</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>133</v>
       </c>
@@ -5358,8 +5637,18 @@
       <c r="E119" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G119">
+        <v>346</v>
+      </c>
+      <c r="H119">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="I119">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J119</f>
+        <v>15.28</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -5375,8 +5664,18 @@
       <c r="E120" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G120">
+        <v>346</v>
+      </c>
+      <c r="H120">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="I120">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J120</f>
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -5392,8 +5691,18 @@
       <c r="E121" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G121">
+        <v>346</v>
+      </c>
+      <c r="H121">
+        <v>12.35</v>
+      </c>
+      <c r="I121">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J121</f>
+        <v>18.86</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>136</v>
       </c>
@@ -5409,8 +5718,18 @@
       <c r="E122" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G122">
+        <v>346</v>
+      </c>
+      <c r="H122">
+        <v>12</v>
+      </c>
+      <c r="I122">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J122</f>
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -5426,8 +5745,18 @@
       <c r="E123" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G123">
+        <v>346</v>
+      </c>
+      <c r="H123">
+        <v>11.33</v>
+      </c>
+      <c r="I123">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J123</f>
+        <v>13.88</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -5443,8 +5772,18 @@
       <c r="E124" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G124">
+        <v>346</v>
+      </c>
+      <c r="H124">
+        <v>14.49</v>
+      </c>
+      <c r="I124">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J124</f>
+        <v>11.36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -5460,8 +5799,18 @@
       <c r="E125" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G125">
+        <v>346</v>
+      </c>
+      <c r="H125">
+        <v>22.01</v>
+      </c>
+      <c r="I125">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J125</f>
+        <v>30.45</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -5477,8 +5826,18 @@
       <c r="E126" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G126">
+        <v>346</v>
+      </c>
+      <c r="H126">
+        <v>13.57</v>
+      </c>
+      <c r="I126">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J126</f>
+        <v>15.42</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -5494,8 +5853,18 @@
       <c r="E127" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G127">
+        <v>346</v>
+      </c>
+      <c r="H127">
+        <v>26.03</v>
+      </c>
+      <c r="I127">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J127</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -5511,8 +5880,18 @@
       <c r="E128" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G128">
+        <v>346</v>
+      </c>
+      <c r="H128">
+        <v>21.22</v>
+      </c>
+      <c r="I128">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J128</f>
+        <v>26.09</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -5528,8 +5907,18 @@
       <c r="E129" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G129">
+        <v>346</v>
+      </c>
+      <c r="H129">
+        <v>18.05</v>
+      </c>
+      <c r="I129">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J129</f>
+        <v>30.42</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -5545,8 +5934,18 @@
       <c r="E130" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G130">
+        <v>346</v>
+      </c>
+      <c r="H130">
+        <v>28.99</v>
+      </c>
+      <c r="I130">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J130</f>
+        <v>30.87</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -5562,8 +5961,18 @@
       <c r="E131" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G131">
+        <v>346</v>
+      </c>
+      <c r="H131">
+        <v>20.85</v>
+      </c>
+      <c r="I131">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J131</f>
+        <v>25.94</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -5579,8 +5988,18 @@
       <c r="E132" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G132">
+        <v>346</v>
+      </c>
+      <c r="H132">
+        <v>23.8</v>
+      </c>
+      <c r="I132">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J132</f>
+        <v>19.55</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -5596,8 +6015,18 @@
       <c r="E133" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G133">
+        <v>346</v>
+      </c>
+      <c r="H133">
+        <v>21.79</v>
+      </c>
+      <c r="I133">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J133</f>
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -5613,8 +6042,18 @@
       <c r="E134" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G134">
+        <v>346</v>
+      </c>
+      <c r="H134">
+        <v>16.010000000000002</v>
+      </c>
+      <c r="I134">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J134</f>
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -5630,8 +6069,18 @@
       <c r="E135" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G135">
+        <v>346</v>
+      </c>
+      <c r="H135">
+        <v>13.14</v>
+      </c>
+      <c r="I135">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J135</f>
+        <v>19.419999999999998</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -5647,8 +6096,18 @@
       <c r="E136" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G136">
+        <v>346</v>
+      </c>
+      <c r="H136">
+        <v>10.73</v>
+      </c>
+      <c r="I136">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J136</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -5664,8 +6123,18 @@
       <c r="E137" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G137">
+        <v>346</v>
+      </c>
+      <c r="H137">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="I137">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J137</f>
+        <v>17.32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -5681,8 +6150,18 @@
       <c r="E138" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G138">
+        <v>346</v>
+      </c>
+      <c r="H138">
+        <v>10.89</v>
+      </c>
+      <c r="I138">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J138</f>
+        <v>17.88</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -5698,8 +6177,18 @@
       <c r="E139" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G139">
+        <v>346</v>
+      </c>
+      <c r="H139">
+        <v>22.02</v>
+      </c>
+      <c r="I139">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J139</f>
+        <v>24.21</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -5715,8 +6204,18 @@
       <c r="E140" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G140">
+        <v>346</v>
+      </c>
+      <c r="H140">
+        <v>22.04</v>
+      </c>
+      <c r="I140">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J140</f>
+        <v>26.44</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -5732,8 +6231,18 @@
       <c r="E141" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G141">
+        <v>346</v>
+      </c>
+      <c r="H141">
+        <v>10.85</v>
+      </c>
+      <c r="I141">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J141</f>
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -5749,8 +6258,18 @@
       <c r="E142" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G142">
+        <v>346</v>
+      </c>
+      <c r="H142">
+        <v>29.59</v>
+      </c>
+      <c r="I142">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J142</f>
+        <v>42.38</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -5766,8 +6285,18 @@
       <c r="E143" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G143">
+        <v>346</v>
+      </c>
+      <c r="H143">
+        <v>28.61</v>
+      </c>
+      <c r="I143">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J143</f>
+        <v>26.44</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>158</v>
       </c>
@@ -5783,8 +6312,18 @@
       <c r="E144" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G144">
+        <v>346</v>
+      </c>
+      <c r="H144">
+        <v>12.24</v>
+      </c>
+      <c r="I144">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J144</f>
+        <v>13.55</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>159</v>
       </c>
@@ -5800,8 +6339,18 @@
       <c r="E145" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G145">
+        <v>346</v>
+      </c>
+      <c r="H145">
+        <v>10.38</v>
+      </c>
+      <c r="I145">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J145</f>
+        <v>12.57</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>160</v>
       </c>
@@ -5817,8 +6366,18 @@
       <c r="E146" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G146">
+        <v>346</v>
+      </c>
+      <c r="H146">
+        <v>30.71</v>
+      </c>
+      <c r="I146">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J146</f>
+        <v>36.92</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -5834,8 +6393,18 @@
       <c r="E147" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G147">
+        <v>346</v>
+      </c>
+      <c r="H147">
+        <v>9.07</v>
+      </c>
+      <c r="I147">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J147</f>
+        <v>10.19</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -5851,8 +6420,18 @@
       <c r="E148" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G148">
+        <v>346</v>
+      </c>
+      <c r="H148">
+        <v>14.79</v>
+      </c>
+      <c r="I148">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J148</f>
+        <v>16.079999999999998</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -5868,8 +6447,18 @@
       <c r="E149" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G149">
+        <v>346</v>
+      </c>
+      <c r="H149">
+        <v>20.72</v>
+      </c>
+      <c r="I149">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J149</f>
+        <v>24.68</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -5885,8 +6474,18 @@
       <c r="E150" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G150">
+        <v>346</v>
+      </c>
+      <c r="H150">
+        <v>26.72</v>
+      </c>
+      <c r="I150">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J150</f>
+        <v>25.05</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -5902,8 +6501,18 @@
       <c r="E151" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G151">
+        <v>346</v>
+      </c>
+      <c r="H151">
+        <v>15.68</v>
+      </c>
+      <c r="I151">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J151</f>
+        <v>17.010000000000002</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>166</v>
       </c>
@@ -5919,8 +6528,18 @@
       <c r="E152" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G152">
+        <v>346</v>
+      </c>
+      <c r="H152">
+        <v>14.26</v>
+      </c>
+      <c r="I152">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J152</f>
+        <v>15.54</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>167</v>
       </c>
@@ -5936,8 +6555,18 @@
       <c r="E153" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G153">
+        <v>346</v>
+      </c>
+      <c r="H153">
+        <v>9.85</v>
+      </c>
+      <c r="I153">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J153</f>
+        <v>15.46</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>168</v>
       </c>
@@ -5953,8 +6582,18 @@
       <c r="E154" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G154">
+        <v>346</v>
+      </c>
+      <c r="H154">
+        <v>15.71</v>
+      </c>
+      <c r="I154">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J154</f>
+        <v>16.79</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>169</v>
       </c>
@@ -5970,8 +6609,18 @@
       <c r="E155" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G155">
+        <v>346</v>
+      </c>
+      <c r="H155" s="2">
+        <v>32.49</v>
+      </c>
+      <c r="I155">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J155</f>
+        <v>34.24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>170</v>
       </c>
@@ -5987,8 +6636,18 @@
       <c r="E156" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G156">
+        <v>346</v>
+      </c>
+      <c r="H156">
+        <v>33.08</v>
+      </c>
+      <c r="I156">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J156</f>
+        <v>32.64</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -6004,8 +6663,18 @@
       <c r="E157" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G157">
+        <v>346</v>
+      </c>
+      <c r="H157" s="2">
+        <v>15.44</v>
+      </c>
+      <c r="I157">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J157</f>
+        <v>21.89</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -6021,8 +6690,18 @@
       <c r="E158" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G158">
+        <v>346</v>
+      </c>
+      <c r="H158" s="2">
+        <v>16.73</v>
+      </c>
+      <c r="I158">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J158</f>
+        <v>17.98</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -6038,8 +6717,18 @@
       <c r="E159" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G159">
+        <v>346</v>
+      </c>
+      <c r="H159" s="2">
+        <v>30.58</v>
+      </c>
+      <c r="I159">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J159</f>
+        <v>30.64</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -6055,8 +6744,18 @@
       <c r="E160" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G160">
+        <v>346</v>
+      </c>
+      <c r="H160" s="2">
+        <v>35.950000000000003</v>
+      </c>
+      <c r="I160">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J160</f>
+        <v>35.49</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -6072,8 +6771,18 @@
       <c r="E161" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G161">
+        <v>346</v>
+      </c>
+      <c r="H161" s="2">
+        <v>16</v>
+      </c>
+      <c r="I161">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J161</f>
+        <v>15.34</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -6089,8 +6798,18 @@
       <c r="E162" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G162">
+        <v>346</v>
+      </c>
+      <c r="H162">
+        <v>43.62</v>
+      </c>
+      <c r="I162">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J162</f>
+        <v>37.119999999999997</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -6106,8 +6825,18 @@
       <c r="E163" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G163">
+        <v>346</v>
+      </c>
+      <c r="H163">
+        <v>9.76</v>
+      </c>
+      <c r="I163">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J163</f>
+        <v>19.72</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -6123,8 +6852,18 @@
       <c r="E164" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G164">
+        <v>346</v>
+      </c>
+      <c r="H164">
+        <v>33.47</v>
+      </c>
+      <c r="I164">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J164</f>
+        <v>21.419999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -6140,8 +6879,18 @@
       <c r="E165" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G165">
+        <v>346</v>
+      </c>
+      <c r="H165">
+        <v>33.18</v>
+      </c>
+      <c r="I165">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J165</f>
+        <v>21.57</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -6157,8 +6906,18 @@
       <c r="E166" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G166">
+        <v>346</v>
+      </c>
+      <c r="H166">
+        <v>14.26</v>
+      </c>
+      <c r="I166">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J166</f>
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>181</v>
       </c>
@@ -6174,8 +6933,18 @@
       <c r="E167" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G167">
+        <v>346</v>
+      </c>
+      <c r="H167">
+        <v>25.5</v>
+      </c>
+      <c r="I167">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J167</f>
+        <v>30.03</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>182</v>
       </c>
@@ -6191,8 +6960,18 @@
       <c r="E168" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G168">
+        <v>346</v>
+      </c>
+      <c r="H168">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="I168">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J168</f>
+        <v>11.33</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>183</v>
       </c>
@@ -6208,8 +6987,18 @@
       <c r="E169" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G169">
+        <v>346</v>
+      </c>
+      <c r="H169">
+        <v>46.67</v>
+      </c>
+      <c r="I169">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J169</f>
+        <v>39.270000000000003</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>184</v>
       </c>
@@ -6225,8 +7014,18 @@
       <c r="E170" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G170">
+        <v>346</v>
+      </c>
+      <c r="H170">
+        <v>10.8</v>
+      </c>
+      <c r="I170">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J170</f>
+        <v>15.29</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>185</v>
       </c>
@@ -6242,8 +7041,18 @@
       <c r="E171" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G171">
+        <v>346</v>
+      </c>
+      <c r="H171">
+        <v>18.739999999999998</v>
+      </c>
+      <c r="I171">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J171</f>
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>186</v>
       </c>
@@ -6259,8 +7068,18 @@
       <c r="E172" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G172">
+        <v>346</v>
+      </c>
+      <c r="H172">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="I172">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J172</f>
+        <v>11.67</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>187</v>
       </c>
@@ -6276,8 +7095,18 @@
       <c r="E173" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G173">
+        <v>346</v>
+      </c>
+      <c r="H173">
+        <v>22.69</v>
+      </c>
+      <c r="I173">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J173</f>
+        <v>27.07</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>188</v>
       </c>
@@ -6293,8 +7122,18 @@
       <c r="E174" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G174">
+        <v>346</v>
+      </c>
+      <c r="H174">
+        <v>10.23</v>
+      </c>
+      <c r="I174">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J174</f>
+        <v>35.24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>189</v>
       </c>
@@ -6310,8 +7149,18 @@
       <c r="E175" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G175">
+        <v>346</v>
+      </c>
+      <c r="H175">
+        <v>34.119999999999997</v>
+      </c>
+      <c r="I175">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J175</f>
+        <v>34.299999999999997</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -6327,8 +7176,18 @@
       <c r="E176" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G176">
+        <v>346</v>
+      </c>
+      <c r="H176">
+        <v>17.059999999999999</v>
+      </c>
+      <c r="I176">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J176</f>
+        <v>27.62</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -6344,8 +7203,18 @@
       <c r="E177" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G177">
+        <v>346</v>
+      </c>
+      <c r="H177">
+        <v>10.31</v>
+      </c>
+      <c r="I177">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J177</f>
+        <v>14.48</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -6361,8 +7230,18 @@
       <c r="E178" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G178">
+        <v>346</v>
+      </c>
+      <c r="H178">
+        <v>11.92</v>
+      </c>
+      <c r="I178">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J178</f>
+        <v>14.75</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>193</v>
       </c>
@@ -6378,8 +7257,18 @@
       <c r="E179" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G179">
+        <v>346</v>
+      </c>
+      <c r="H179">
+        <v>21.1</v>
+      </c>
+      <c r="I179">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J179</f>
+        <v>19.309999999999999</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -6395,8 +7284,18 @@
       <c r="E180" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G180">
+        <v>346</v>
+      </c>
+      <c r="H180">
+        <v>16.850000000000001</v>
+      </c>
+      <c r="I180">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J180</f>
+        <v>19.18</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>195</v>
       </c>
@@ -6411,6 +7310,16 @@
       </c>
       <c r="E181" t="s">
         <v>106</v>
+      </c>
+      <c r="G181">
+        <v>346</v>
+      </c>
+      <c r="H181">
+        <v>9.41</v>
+      </c>
+      <c r="I181">
+        <f ca="1">Table1[[#This Row],[belowGroundWeight]]-J181</f>
+        <v>10.11</v>
       </c>
     </row>
     <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -6429,6 +7338,15 @@
       <c r="E182" t="s">
         <v>198</v>
       </c>
+      <c r="G182">
+        <v>346</v>
+      </c>
+      <c r="H182" s="2">
+        <v>59.53</v>
+      </c>
+      <c r="I182">
+        <v>96.99</v>
+      </c>
     </row>
     <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
@@ -6446,6 +7364,15 @@
       <c r="E183" t="s">
         <v>198</v>
       </c>
+      <c r="G183">
+        <v>346</v>
+      </c>
+      <c r="H183" s="2">
+        <v>40.6</v>
+      </c>
+      <c r="I183" s="2">
+        <v>69.02</v>
+      </c>
     </row>
     <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
@@ -6463,6 +7390,15 @@
       <c r="E184" t="s">
         <v>198</v>
       </c>
+      <c r="G184">
+        <v>346</v>
+      </c>
+      <c r="H184" s="2">
+        <v>19.579999999999998</v>
+      </c>
+      <c r="I184" s="2">
+        <v>49.56</v>
+      </c>
     </row>
     <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
@@ -6480,6 +7416,15 @@
       <c r="E185" t="s">
         <v>198</v>
       </c>
+      <c r="G185">
+        <v>346</v>
+      </c>
+      <c r="H185" s="2">
+        <v>6.74</v>
+      </c>
+      <c r="I185" s="2">
+        <v>23.77</v>
+      </c>
     </row>
     <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
@@ -6497,6 +7442,15 @@
       <c r="E186" t="s">
         <v>198</v>
       </c>
+      <c r="G186">
+        <v>346</v>
+      </c>
+      <c r="H186" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="I186" s="2">
+        <v>54.95</v>
+      </c>
     </row>
     <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
@@ -6744,6 +7698,15 @@
       <c r="E197" t="s">
         <v>198</v>
       </c>
+      <c r="G197">
+        <v>346</v>
+      </c>
+      <c r="H197">
+        <v>21.71</v>
+      </c>
+      <c r="I197">
+        <v>20.63</v>
+      </c>
     </row>
     <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
@@ -6761,6 +7724,15 @@
       <c r="E198" t="s">
         <v>198</v>
       </c>
+      <c r="G198">
+        <v>346</v>
+      </c>
+      <c r="H198">
+        <v>24.34</v>
+      </c>
+      <c r="I198">
+        <v>49.52</v>
+      </c>
     </row>
     <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
@@ -6778,6 +7750,15 @@
       <c r="E199" t="s">
         <v>198</v>
       </c>
+      <c r="G199">
+        <v>346</v>
+      </c>
+      <c r="H199">
+        <v>36.729999999999997</v>
+      </c>
+      <c r="I199">
+        <v>62.22</v>
+      </c>
     </row>
     <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
@@ -6795,6 +7776,15 @@
       <c r="E200" t="s">
         <v>198</v>
       </c>
+      <c r="G200">
+        <v>346</v>
+      </c>
+      <c r="H200">
+        <v>16.940000000000001</v>
+      </c>
+      <c r="I200">
+        <v>41.39</v>
+      </c>
     </row>
     <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
@@ -6812,6 +7802,15 @@
       <c r="E201" t="s">
         <v>198</v>
       </c>
+      <c r="G201">
+        <v>346</v>
+      </c>
+      <c r="H201">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="I201">
+        <v>24.83</v>
+      </c>
     </row>
     <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
@@ -7059,6 +8058,15 @@
       <c r="E212" t="s">
         <v>198</v>
       </c>
+      <c r="G212">
+        <v>346</v>
+      </c>
+      <c r="H212">
+        <v>24.32</v>
+      </c>
+      <c r="I212">
+        <v>53.81</v>
+      </c>
     </row>
     <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
@@ -7076,6 +8084,15 @@
       <c r="E213" t="s">
         <v>198</v>
       </c>
+      <c r="G213">
+        <v>346</v>
+      </c>
+      <c r="H213">
+        <v>10.3</v>
+      </c>
+      <c r="I213">
+        <v>25.08</v>
+      </c>
     </row>
     <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
@@ -7093,6 +8110,15 @@
       <c r="E214" t="s">
         <v>198</v>
       </c>
+      <c r="G214">
+        <v>346</v>
+      </c>
+      <c r="H214">
+        <v>24.25</v>
+      </c>
+      <c r="I214">
+        <v>41.9</v>
+      </c>
     </row>
     <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
@@ -7110,6 +8136,15 @@
       <c r="E215" t="s">
         <v>198</v>
       </c>
+      <c r="G215">
+        <v>346</v>
+      </c>
+      <c r="H215">
+        <v>17.16</v>
+      </c>
+      <c r="I215">
+        <v>36.369999999999997</v>
+      </c>
     </row>
     <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
@@ -7127,6 +8162,15 @@
       <c r="E216" t="s">
         <v>198</v>
       </c>
+      <c r="G216">
+        <v>346</v>
+      </c>
+      <c r="H216">
+        <v>15.64</v>
+      </c>
+      <c r="I216">
+        <v>26.44</v>
+      </c>
     </row>
     <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
@@ -7374,6 +8418,15 @@
       <c r="E227" t="s">
         <v>198</v>
       </c>
+      <c r="G227">
+        <v>346</v>
+      </c>
+      <c r="H227">
+        <v>13.79</v>
+      </c>
+      <c r="I227">
+        <v>43.77</v>
+      </c>
     </row>
     <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
@@ -7391,6 +8444,15 @@
       <c r="E228" t="s">
         <v>198</v>
       </c>
+      <c r="G228">
+        <v>346</v>
+      </c>
+      <c r="H228">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="I228">
+        <v>19.14</v>
+      </c>
     </row>
     <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
@@ -7408,6 +8470,15 @@
       <c r="E229" t="s">
         <v>198</v>
       </c>
+      <c r="G229">
+        <v>346</v>
+      </c>
+      <c r="H229">
+        <v>36.82</v>
+      </c>
+      <c r="I229">
+        <v>69.599999999999994</v>
+      </c>
     </row>
     <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
@@ -7425,6 +8496,15 @@
       <c r="E230" t="s">
         <v>198</v>
       </c>
+      <c r="G230">
+        <v>346</v>
+      </c>
+      <c r="H230">
+        <v>11.29</v>
+      </c>
+      <c r="I230">
+        <v>30.15</v>
+      </c>
     </row>
     <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
@@ -7442,6 +8522,15 @@
       <c r="E231" t="s">
         <v>198</v>
       </c>
+      <c r="G231">
+        <v>346</v>
+      </c>
+      <c r="H231">
+        <v>8.39</v>
+      </c>
+      <c r="I231">
+        <v>8.56</v>
+      </c>
     </row>
     <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
@@ -7689,6 +8778,15 @@
       <c r="E242" t="s">
         <v>198</v>
       </c>
+      <c r="G242">
+        <v>346</v>
+      </c>
+      <c r="H242">
+        <v>29.7</v>
+      </c>
+      <c r="I242">
+        <v>61.49</v>
+      </c>
     </row>
     <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
@@ -7706,6 +8804,15 @@
       <c r="E243" t="s">
         <v>198</v>
       </c>
+      <c r="G243">
+        <v>346</v>
+      </c>
+      <c r="H243">
+        <v>30.06</v>
+      </c>
+      <c r="I243">
+        <v>41.42</v>
+      </c>
     </row>
     <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
@@ -7723,6 +8830,15 @@
       <c r="E244" t="s">
         <v>198</v>
       </c>
+      <c r="G244">
+        <v>346</v>
+      </c>
+      <c r="H244">
+        <v>13.81</v>
+      </c>
+      <c r="I244">
+        <v>44.69</v>
+      </c>
     </row>
     <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
@@ -7740,6 +8856,15 @@
       <c r="E245" t="s">
         <v>198</v>
       </c>
+      <c r="G245">
+        <v>346</v>
+      </c>
+      <c r="H245">
+        <v>7.9</v>
+      </c>
+      <c r="I245">
+        <v>21.34</v>
+      </c>
     </row>
     <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
@@ -7757,6 +8882,15 @@
       <c r="E246" t="s">
         <v>198</v>
       </c>
+      <c r="G246">
+        <v>346</v>
+      </c>
+      <c r="H246">
+        <v>26.6</v>
+      </c>
+      <c r="I246">
+        <v>16.14</v>
+      </c>
     </row>
     <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
@@ -8004,6 +9138,15 @@
       <c r="E257" t="s">
         <v>198</v>
       </c>
+      <c r="G257">
+        <v>346</v>
+      </c>
+      <c r="H257">
+        <v>16.73</v>
+      </c>
+      <c r="I257">
+        <v>36.369999999999997</v>
+      </c>
     </row>
     <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
@@ -8021,6 +9164,15 @@
       <c r="E258" t="s">
         <v>198</v>
       </c>
+      <c r="G258">
+        <v>346</v>
+      </c>
+      <c r="H258">
+        <v>23.87</v>
+      </c>
+      <c r="I258">
+        <v>42.48</v>
+      </c>
     </row>
     <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
@@ -8038,6 +9190,15 @@
       <c r="E259" t="s">
         <v>198</v>
       </c>
+      <c r="G259">
+        <v>346</v>
+      </c>
+      <c r="H259">
+        <v>16.87</v>
+      </c>
+      <c r="I259">
+        <v>37.1</v>
+      </c>
     </row>
     <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
@@ -8055,6 +9216,15 @@
       <c r="E260" t="s">
         <v>198</v>
       </c>
+      <c r="G260">
+        <v>346</v>
+      </c>
+      <c r="H260">
+        <v>15.13</v>
+      </c>
+      <c r="I260">
+        <v>34.64</v>
+      </c>
     </row>
     <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
@@ -8072,6 +9242,15 @@
       <c r="E261" t="s">
         <v>198</v>
       </c>
+      <c r="G261">
+        <v>346</v>
+      </c>
+      <c r="H261">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="I261">
+        <v>49.72</v>
+      </c>
     </row>
     <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
@@ -8322,8 +9501,11 @@
       <c r="E272" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G272" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>291</v>
       </c>
@@ -8339,8 +9521,11 @@
       <c r="E273" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G273" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>292</v>
       </c>
@@ -8356,8 +9541,11 @@
       <c r="E274" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G274" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>293</v>
       </c>
@@ -8373,8 +9561,11 @@
       <c r="E275" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G275" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>294</v>
       </c>
@@ -8390,8 +9581,11 @@
       <c r="E276" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G276" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>295</v>
       </c>
@@ -8408,7 +9602,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>296</v>
       </c>
@@ -8425,7 +9619,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>297</v>
       </c>
@@ -8442,7 +9636,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>298</v>
       </c>
@@ -8459,7 +9653,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>299</v>
       </c>
@@ -8476,7 +9670,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>300</v>
       </c>
@@ -8493,7 +9687,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>301</v>
       </c>
@@ -8510,7 +9704,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>302</v>
       </c>
@@ -8527,7 +9721,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>303</v>
       </c>
@@ -8544,7 +9738,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="286" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>304</v>
       </c>
@@ -8560,8 +9754,11 @@
       <c r="E286" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G286" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>305</v>
       </c>
@@ -8577,8 +9774,11 @@
       <c r="E287" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G287" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>306</v>
       </c>
@@ -8594,8 +9794,11 @@
       <c r="E288" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="289" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G288" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>307</v>
       </c>
@@ -8611,8 +9814,11 @@
       <c r="E289" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="290" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G289" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>308</v>
       </c>
@@ -8628,8 +9834,11 @@
       <c r="E290" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="291" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G290" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>309</v>
       </c>
@@ -8646,7 +9855,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>310</v>
       </c>
@@ -8663,7 +9872,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="293" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>311</v>
       </c>
@@ -8680,7 +9889,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="294" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>312</v>
       </c>
@@ -8697,7 +9906,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="295" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>313</v>
       </c>
@@ -8714,7 +9923,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="296" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
@@ -8731,7 +9940,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="297" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
@@ -8748,7 +9957,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="298" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
@@ -8765,7 +9974,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="299" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
@@ -8782,7 +9991,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="300" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -8799,7 +10008,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="301" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>319</v>
       </c>
@@ -8815,8 +10024,11 @@
       <c r="E301" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G301" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>320</v>
       </c>
@@ -8832,8 +10044,11 @@
       <c r="E302" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="303" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G302" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>321</v>
       </c>
@@ -8849,8 +10064,11 @@
       <c r="E303" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="304" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G303" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>322</v>
       </c>
@@ -8866,8 +10084,11 @@
       <c r="E304" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="305" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G304" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>323</v>
       </c>
@@ -8883,8 +10104,11 @@
       <c r="E305" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="306" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G305" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>324</v>
       </c>
@@ -8901,7 +10125,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="307" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>325</v>
       </c>
@@ -8918,7 +10142,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="308" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>326</v>
       </c>
@@ -8935,7 +10159,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="309" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>327</v>
       </c>
@@ -8952,7 +10176,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="310" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>328</v>
       </c>
@@ -8969,7 +10193,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="311" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>329</v>
       </c>
@@ -8986,7 +10210,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="312" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>330</v>
       </c>
@@ -9003,7 +10227,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="313" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>331</v>
       </c>
@@ -9020,7 +10244,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="314" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>332</v>
       </c>
@@ -9037,7 +10261,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="315" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>333</v>
       </c>
@@ -9054,7 +10278,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="316" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>334</v>
       </c>
@@ -9070,8 +10294,11 @@
       <c r="E316" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="317" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G316" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>335</v>
       </c>
@@ -9087,8 +10314,11 @@
       <c r="E317" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="318" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G317" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>336</v>
       </c>
@@ -9104,8 +10334,11 @@
       <c r="E318" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="319" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G318" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>337</v>
       </c>
@@ -9121,8 +10354,11 @@
       <c r="E319" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="320" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G319" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>338</v>
       </c>
@@ -9138,8 +10374,11 @@
       <c r="E320" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="321" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G320" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>339</v>
       </c>
@@ -9156,7 +10395,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="322" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>340</v>
       </c>
@@ -9173,7 +10412,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="323" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>341</v>
       </c>
@@ -9190,7 +10429,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="324" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>342</v>
       </c>
@@ -9207,7 +10446,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="325" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -9224,7 +10463,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="326" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>344</v>
       </c>
@@ -9241,7 +10480,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="327" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>345</v>
       </c>
@@ -9258,7 +10497,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="328" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>346</v>
       </c>
@@ -9275,7 +10514,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="329" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>347</v>
       </c>
@@ -9291,8 +10530,11 @@
       <c r="E329" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="330" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G329" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>348</v>
       </c>
@@ -9308,8 +10550,11 @@
       <c r="E330" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="331" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G330" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>349</v>
       </c>
@@ -9325,8 +10570,11 @@
       <c r="E331" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="332" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G331" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>350</v>
       </c>
@@ -9342,8 +10590,11 @@
       <c r="E332" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="333" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G332" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>351</v>
       </c>
@@ -9359,8 +10610,11 @@
       <c r="E333" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="334" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G333" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>352</v>
       </c>
@@ -9377,7 +10631,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="335" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>353</v>
       </c>
@@ -9394,7 +10648,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="336" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>354</v>
       </c>
@@ -9411,7 +10665,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="337" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>355</v>
       </c>
@@ -9428,7 +10682,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="338" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>356</v>
       </c>
@@ -9445,7 +10699,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="339" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>357</v>
       </c>
@@ -9462,7 +10716,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="340" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>358</v>
       </c>
@@ -9479,7 +10733,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="341" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>359</v>
       </c>
@@ -9496,7 +10750,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="342" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>360</v>
       </c>
@@ -9513,7 +10767,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="343" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>361</v>
       </c>
@@ -9530,7 +10784,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="344" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -9546,8 +10800,11 @@
       <c r="E344" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="345" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G344" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>363</v>
       </c>
@@ -9563,8 +10820,11 @@
       <c r="E345" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="346" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G345" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>364</v>
       </c>
@@ -9580,8 +10840,11 @@
       <c r="E346" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="347" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G346" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>365</v>
       </c>
@@ -9597,8 +10860,11 @@
       <c r="E347" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="348" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G347" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>366</v>
       </c>
@@ -9614,8 +10880,11 @@
       <c r="E348" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="349" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G348" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>367</v>
       </c>
@@ -9632,7 +10901,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="350" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>368</v>
       </c>
@@ -9649,7 +10918,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="351" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>369</v>
       </c>
@@ -9666,7 +10935,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="352" spans="1:5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>370</v>
       </c>
@@ -13780,7 +15049,7 @@
         <v>38.96</v>
       </c>
     </row>
-    <row r="528" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="528" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A528" t="s">
         <v>550</v>
       </c>
@@ -13797,7 +15066,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="529" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="529" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
         <v>553</v>
       </c>
@@ -13820,7 +15089,7 @@
         <v>47.81</v>
       </c>
     </row>
-    <row r="530" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="530" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A530" t="s">
         <v>554</v>
       </c>
@@ -13836,10 +15105,8 @@
       <c r="E530" t="s">
         <v>552</v>
       </c>
-      <c r="H530" s="2"/>
-      <c r="I530" s="2"/>
-    </row>
-    <row r="531" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="531" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A531" t="s">
         <v>555</v>
       </c>
@@ -13862,7 +15129,7 @@
         <v>18.84</v>
       </c>
     </row>
-    <row r="532" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="532" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A532" t="s">
         <v>556</v>
       </c>
@@ -13885,7 +15152,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="533" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="533" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A533" t="s">
         <v>557</v>
       </c>
@@ -13908,7 +15175,7 @@
         <v>46.47</v>
       </c>
     </row>
-    <row r="534" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="534" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A534" t="s">
         <v>558</v>
       </c>
@@ -13931,7 +15198,7 @@
         <v>58.75</v>
       </c>
     </row>
-    <row r="535" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="535" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
         <v>559</v>
       </c>
@@ -13954,7 +15221,7 @@
         <v>40.49</v>
       </c>
     </row>
-    <row r="536" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="536" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
         <v>560</v>
       </c>
@@ -13977,7 +15244,7 @@
         <v>22.01</v>
       </c>
     </row>
-    <row r="537" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="537" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A537" t="s">
         <v>561</v>
       </c>
@@ -14000,7 +15267,7 @@
         <v>38.18</v>
       </c>
     </row>
-    <row r="538" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="538" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A538" t="s">
         <v>562</v>
       </c>
@@ -14017,7 +15284,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="539" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="539" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A539" t="s">
         <v>563</v>
       </c>
@@ -14040,7 +15307,7 @@
         <v>15.57</v>
       </c>
     </row>
-    <row r="540" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="540" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A540" t="s">
         <v>564</v>
       </c>
@@ -14057,7 +15324,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="541" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="541" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A541" t="s">
         <v>565</v>
       </c>
@@ -14080,7 +15347,7 @@
         <v>11.61</v>
       </c>
     </row>
-    <row r="542" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="542" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A542" t="s">
         <v>566</v>
       </c>
@@ -14103,7 +15370,7 @@
         <v>25.56</v>
       </c>
     </row>
-    <row r="543" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="543" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A543" t="s">
         <v>567</v>
       </c>
@@ -14120,7 +15387,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="544" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="544" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A544" t="s">
         <v>568</v>
       </c>
@@ -14143,7 +15410,7 @@
         <v>24.46</v>
       </c>
     </row>
-    <row r="545" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="545" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A545" t="s">
         <v>569</v>
       </c>
@@ -14166,7 +15433,7 @@
         <v>44.88</v>
       </c>
     </row>
-    <row r="546" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="546" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A546" t="s">
         <v>570</v>
       </c>
@@ -14189,7 +15456,7 @@
         <v>23.17</v>
       </c>
     </row>
-    <row r="547" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="547" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A547" t="s">
         <v>571</v>
       </c>
@@ -14212,7 +15479,7 @@
         <v>39.979999999999997</v>
       </c>
     </row>
-    <row r="548" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="548" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A548" t="s">
         <v>572</v>
       </c>
@@ -14235,7 +15502,7 @@
         <v>27.39</v>
       </c>
     </row>
-    <row r="549" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="549" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A549" t="s">
         <v>573</v>
       </c>
@@ -14258,7 +15525,7 @@
         <v>64.31</v>
       </c>
     </row>
-    <row r="550" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="550" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A550" t="s">
         <v>574</v>
       </c>
@@ -14281,7 +15548,7 @@
         <v>63.08</v>
       </c>
     </row>
-    <row r="551" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="551" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A551" t="s">
         <v>575</v>
       </c>
@@ -14304,7 +15571,7 @@
         <v>14.76</v>
       </c>
     </row>
-    <row r="552" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="552" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
         <v>576</v>
       </c>
@@ -14321,7 +15588,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="553" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="553" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
         <v>577</v>
       </c>
@@ -14344,7 +15611,7 @@
         <v>36.450000000000003</v>
       </c>
     </row>
-    <row r="554" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="554" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
         <v>578</v>
       </c>
@@ -14367,7 +15634,7 @@
         <v>45.38</v>
       </c>
     </row>
-    <row r="555" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="555" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A555" t="s">
         <v>579</v>
       </c>
@@ -14390,7 +15657,7 @@
         <v>52.68</v>
       </c>
     </row>
-    <row r="556" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="556" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A556" t="s">
         <v>580</v>
       </c>
@@ -14413,7 +15680,7 @@
         <v>38.04</v>
       </c>
     </row>
-    <row r="557" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="557" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A557" t="s">
         <v>581</v>
       </c>
@@ -14430,7 +15697,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="558" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="558" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A558" t="s">
         <v>582</v>
       </c>
@@ -14453,7 +15720,7 @@
         <v>34.21</v>
       </c>
     </row>
-    <row r="559" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="559" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A559" t="s">
         <v>583</v>
       </c>
@@ -14477,7 +15744,7 @@
         <v>50.05</v>
       </c>
     </row>
-    <row r="560" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="560" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A560" t="s">
         <v>584</v>
       </c>
@@ -14494,7 +15761,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="561" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>585</v>
       </c>
@@ -14511,7 +15778,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="562" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>586</v>
       </c>
@@ -14528,7 +15795,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="563" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A563" t="s">
         <v>587</v>
       </c>
@@ -14551,7 +15818,7 @@
         <v>48.09</v>
       </c>
     </row>
-    <row r="564" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A564" t="s">
         <v>588</v>
       </c>
@@ -14568,7 +15835,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="565" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A565" t="s">
         <v>589</v>
       </c>
@@ -14591,7 +15858,7 @@
         <v>49.77</v>
       </c>
     </row>
-    <row r="566" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
         <v>590</v>
       </c>
@@ -14614,7 +15881,7 @@
         <v>32.090000000000003</v>
       </c>
     </row>
-    <row r="567" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A567" t="s">
         <v>591</v>
       </c>
@@ -14637,7 +15904,7 @@
         <v>39.06</v>
       </c>
     </row>
-    <row r="568" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A568" t="s">
         <v>592</v>
       </c>
@@ -14661,7 +15928,7 @@
         <v>51.09</v>
       </c>
     </row>
-    <row r="569" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A569" t="s">
         <v>593</v>
       </c>
@@ -14678,7 +15945,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="570" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="570" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>594</v>
       </c>
@@ -14701,7 +15968,7 @@
         <v>31.86</v>
       </c>
     </row>
-    <row r="571" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>595</v>
       </c>
@@ -14724,7 +15991,7 @@
         <v>59.87</v>
       </c>
     </row>
-    <row r="572" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
         <v>596</v>
       </c>
@@ -14747,7 +16014,7 @@
         <v>65.760000000000005</v>
       </c>
     </row>
-    <row r="573" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
         <v>597</v>
       </c>
@@ -14770,7 +16037,7 @@
         <v>25.87</v>
       </c>
     </row>
-    <row r="574" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>598</v>
       </c>
@@ -14787,7 +16054,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="575" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A575" t="s">
         <v>599</v>
       </c>
@@ -14804,7 +16071,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="576" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A576" t="s">
         <v>600</v>
       </c>
@@ -14821,7 +16088,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="577" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A577" t="s">
         <v>601</v>
       </c>
@@ -14844,7 +16111,7 @@
         <v>3.04</v>
       </c>
     </row>
-    <row r="578" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A578" t="s">
         <v>602</v>
       </c>
@@ -14867,7 +16134,7 @@
         <v>102.04</v>
       </c>
     </row>
-    <row r="579" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A579" t="s">
         <v>603</v>
       </c>
@@ -14890,7 +16157,7 @@
         <v>60.99</v>
       </c>
     </row>
-    <row r="580" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A580" t="s">
         <v>604</v>
       </c>
@@ -14913,7 +16180,7 @@
         <v>54.2</v>
       </c>
     </row>
-    <row r="581" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="581" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A581" t="s">
         <v>605</v>
       </c>
@@ -14936,7 +16203,7 @@
         <v>49.65</v>
       </c>
     </row>
-    <row r="582" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
         <v>606</v>
       </c>
@@ -14959,7 +16226,7 @@
         <v>3.29</v>
       </c>
     </row>
-    <row r="583" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A583" t="s">
         <v>607</v>
       </c>
@@ -14982,7 +16249,7 @@
         <v>23.04</v>
       </c>
     </row>
-    <row r="584" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
         <v>608</v>
       </c>
@@ -15005,7 +16272,7 @@
         <v>29.88</v>
       </c>
     </row>
-    <row r="585" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
         <v>609</v>
       </c>
@@ -15028,7 +16295,7 @@
         <v>54.6</v>
       </c>
     </row>
-    <row r="586" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="586" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
         <v>610</v>
       </c>
@@ -15051,7 +16318,7 @@
         <v>36.08</v>
       </c>
     </row>
-    <row r="587" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
         <v>611</v>
       </c>
@@ -15068,7 +16335,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="588" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A588" t="s">
         <v>612</v>
       </c>
@@ -15091,7 +16358,7 @@
         <v>42.14</v>
       </c>
     </row>
-    <row r="589" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A589" t="s">
         <v>613</v>
       </c>
@@ -15108,7 +16375,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="590" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A590" t="s">
         <v>614</v>
       </c>
@@ -15125,7 +16392,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="591" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A591" t="s">
         <v>615</v>
       </c>
@@ -15142,7 +16409,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="592" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A592" t="s">
         <v>616</v>
       </c>
@@ -15165,7 +16432,7 @@
         <v>14.62</v>
       </c>
     </row>
-    <row r="593" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="593" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A593" t="s">
         <v>617</v>
       </c>
@@ -15181,14 +16448,14 @@
       <c r="E593" t="s">
         <v>552</v>
       </c>
-      <c r="H593" s="2">
+      <c r="H593">
         <v>24.84</v>
       </c>
-      <c r="I593" s="2">
+      <c r="I593">
         <v>40.42</v>
       </c>
     </row>
-    <row r="594" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="594" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A594" t="s">
         <v>618</v>
       </c>
@@ -15211,7 +16478,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="595" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="595" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A595" t="s">
         <v>619</v>
       </c>
@@ -15228,7 +16495,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="596" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="596" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A596" t="s">
         <v>620</v>
       </c>
@@ -15251,7 +16518,7 @@
         <v>25.61</v>
       </c>
     </row>
-    <row r="597" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="597" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A597" t="s">
         <v>621</v>
       </c>
@@ -15268,7 +16535,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="598" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A598" t="s">
         <v>622</v>
       </c>
@@ -15285,7 +16552,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="599" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="599" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A599" t="s">
         <v>623</v>
       </c>
@@ -15308,7 +16575,7 @@
         <v>30.13</v>
       </c>
     </row>
-    <row r="600" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="600" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
         <v>624</v>
       </c>
@@ -15331,7 +16598,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="601" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="601" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A601" t="s">
         <v>625</v>
       </c>
@@ -15354,7 +16621,7 @@
         <v>15.12</v>
       </c>
     </row>
-    <row r="602" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="602" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A602" t="s">
         <v>626</v>
       </c>
@@ -15377,7 +16644,7 @@
         <v>46.17</v>
       </c>
     </row>
-    <row r="603" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="603" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
         <v>627</v>
       </c>
@@ -15400,7 +16667,7 @@
         <v>36.78</v>
       </c>
     </row>
-    <row r="604" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A604" t="s">
         <v>628</v>
       </c>
@@ -15423,7 +16690,7 @@
         <v>6.78</v>
       </c>
     </row>
-    <row r="605" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="605" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
         <v>629</v>
       </c>
@@ -15446,7 +16713,7 @@
         <v>47.97</v>
       </c>
     </row>
-    <row r="606" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="606" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
         <v>630</v>
       </c>
@@ -15462,9 +16729,8 @@
       <c r="E606" t="s">
         <v>552</v>
       </c>
-      <c r="H606" s="2"/>
-    </row>
-    <row r="607" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="607" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A607" t="s">
         <v>631</v>
       </c>
@@ -15487,7 +16753,7 @@
         <v>29.54</v>
       </c>
     </row>
-    <row r="608" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="608" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A608" t="s">
         <v>632</v>
       </c>
@@ -15510,7 +16776,7 @@
         <v>51.46</v>
       </c>
     </row>
-    <row r="609" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A609" t="s">
         <v>633</v>
       </c>
@@ -15533,7 +16799,7 @@
         <v>28.47</v>
       </c>
     </row>
-    <row r="610" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A610" t="s">
         <v>634</v>
       </c>
@@ -15556,7 +16822,7 @@
         <v>41.69</v>
       </c>
     </row>
-    <row r="611" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A611" t="s">
         <v>635</v>
       </c>
@@ -15579,7 +16845,7 @@
         <v>49.01</v>
       </c>
     </row>
-    <row r="612" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A612" t="s">
         <v>636</v>
       </c>
@@ -15602,7 +16868,7 @@
         <v>38.869999999999997</v>
       </c>
     </row>
-    <row r="613" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>637</v>
       </c>
@@ -15625,7 +16891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="614" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A614" t="s">
         <v>638</v>
       </c>
@@ -15648,7 +16914,7 @@
         <v>28.78</v>
       </c>
     </row>
-    <row r="615" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A615" t="s">
         <v>639</v>
       </c>
@@ -15671,7 +16937,7 @@
         <v>44.41</v>
       </c>
     </row>
-    <row r="616" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A616" t="s">
         <v>640</v>
       </c>
@@ -15694,7 +16960,7 @@
         <v>29.08</v>
       </c>
     </row>
-    <row r="617" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A617" t="s">
         <v>641</v>
       </c>

</xml_diff>

<commit_message>
FINAL TWO BLOCS OF POBA AND EVERYTHING!!
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/biomass.xlsx
+++ b/data/treeMeasurements/biomass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8AC9CC-A322-3044-8819-A04EE48884BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D3FECD-7BDB-8F4C-BFFD-E5C956E3811D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2039,8 +2039,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2116,7 +2116,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2204,9 +2204,14 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I617" totalsRowShown="0">
   <autoFilter ref="A1:I617" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4">
       <filters>
-        <filter val="betula_papyrifera"/>
+        <filter val="populus_balsamifera"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -2505,9 +2510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J617"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A150" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H155" sqref="H155"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H352" sqref="H352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4891,7 +4896,7 @@
         <v>17.54</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>104</v>
       </c>
@@ -4918,7 +4923,7 @@
         <v>19.12</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -4945,7 +4950,7 @@
         <v>12.95</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -4972,7 +4977,7 @@
         <v>16.260000000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>109</v>
       </c>
@@ -4999,7 +5004,7 @@
         <v>25.59</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>110</v>
       </c>
@@ -5026,7 +5031,7 @@
         <v>17.649999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>111</v>
       </c>
@@ -5053,7 +5058,7 @@
         <v>29.51</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>112</v>
       </c>
@@ -5080,7 +5085,7 @@
         <v>26.55</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>113</v>
       </c>
@@ -5107,7 +5112,7 @@
         <v>38.93</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>114</v>
       </c>
@@ -5134,7 +5139,7 @@
         <v>32.869999999999997</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>115</v>
       </c>
@@ -5161,7 +5166,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>116</v>
       </c>
@@ -5188,7 +5193,7 @@
         <v>20.329999999999998</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>117</v>
       </c>
@@ -5215,7 +5220,7 @@
         <v>12.17</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>118</v>
       </c>
@@ -5242,7 +5247,7 @@
         <v>42.11</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -5269,7 +5274,7 @@
         <v>17.18</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>120</v>
       </c>
@@ -5297,7 +5302,7 @@
         <v>17.149999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>121</v>
       </c>
@@ -5324,7 +5329,7 @@
         <v>38.83</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>122</v>
       </c>
@@ -5351,7 +5356,7 @@
         <v>14.95</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -5378,7 +5383,7 @@
         <v>17.559999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>124</v>
       </c>
@@ -5405,7 +5410,7 @@
         <v>12.01</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>125</v>
       </c>
@@ -5432,7 +5437,7 @@
         <v>46.09</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -5459,7 +5464,7 @@
         <v>38.270000000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>127</v>
       </c>
@@ -5486,7 +5491,7 @@
         <v>13.45</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>128</v>
       </c>
@@ -5513,7 +5518,7 @@
         <v>33.840000000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>129</v>
       </c>
@@ -5540,7 +5545,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>130</v>
       </c>
@@ -5567,7 +5572,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>131</v>
       </c>
@@ -5586,7 +5591,7 @@
       <c r="G117">
         <v>346</v>
       </c>
-      <c r="H117" s="2">
+      <c r="H117">
         <v>24.57</v>
       </c>
       <c r="I117">
@@ -5594,7 +5599,7 @@
         <v>27.72</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>132</v>
       </c>
@@ -5621,7 +5626,7 @@
         <v>14.02</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>133</v>
       </c>
@@ -5648,7 +5653,7 @@
         <v>15.28</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>134</v>
       </c>
@@ -5675,7 +5680,7 @@
         <v>9.83</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>135</v>
       </c>
@@ -5702,7 +5707,7 @@
         <v>18.86</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>136</v>
       </c>
@@ -5729,7 +5734,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>137</v>
       </c>
@@ -5756,7 +5761,7 @@
         <v>13.88</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>138</v>
       </c>
@@ -5783,7 +5788,7 @@
         <v>11.36</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>139</v>
       </c>
@@ -5810,7 +5815,7 @@
         <v>30.45</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>140</v>
       </c>
@@ -5837,7 +5842,7 @@
         <v>15.42</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>141</v>
       </c>
@@ -5864,7 +5869,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>142</v>
       </c>
@@ -5891,7 +5896,7 @@
         <v>26.09</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>143</v>
       </c>
@@ -5918,7 +5923,7 @@
         <v>30.42</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>144</v>
       </c>
@@ -5945,7 +5950,7 @@
         <v>30.87</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>145</v>
       </c>
@@ -5972,7 +5977,7 @@
         <v>25.94</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -5999,7 +6004,7 @@
         <v>19.55</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>147</v>
       </c>
@@ -6026,7 +6031,7 @@
         <v>19.11</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>148</v>
       </c>
@@ -6053,7 +6058,7 @@
         <v>13.33</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -6080,7 +6085,7 @@
         <v>19.419999999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -6107,7 +6112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -6134,7 +6139,7 @@
         <v>17.32</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -6161,7 +6166,7 @@
         <v>17.88</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -6188,7 +6193,7 @@
         <v>24.21</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -6215,7 +6220,7 @@
         <v>26.44</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -6242,7 +6247,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -6269,7 +6274,7 @@
         <v>42.38</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -6296,7 +6301,7 @@
         <v>26.44</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>158</v>
       </c>
@@ -6323,7 +6328,7 @@
         <v>13.55</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>159</v>
       </c>
@@ -6350,7 +6355,7 @@
         <v>12.57</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>160</v>
       </c>
@@ -6377,7 +6382,7 @@
         <v>36.92</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -6404,7 +6409,7 @@
         <v>10.19</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -6431,7 +6436,7 @@
         <v>16.079999999999998</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -6458,7 +6463,7 @@
         <v>24.68</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -6485,7 +6490,7 @@
         <v>25.05</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -6512,7 +6517,7 @@
         <v>17.010000000000002</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>166</v>
       </c>
@@ -6539,7 +6544,7 @@
         <v>15.54</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>167</v>
       </c>
@@ -6566,7 +6571,7 @@
         <v>15.46</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>168</v>
       </c>
@@ -6593,7 +6598,7 @@
         <v>16.79</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>169</v>
       </c>
@@ -6612,7 +6617,7 @@
       <c r="G155">
         <v>346</v>
       </c>
-      <c r="H155" s="2">
+      <c r="H155">
         <v>32.49</v>
       </c>
       <c r="I155">
@@ -6620,7 +6625,7 @@
         <v>34.24</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>170</v>
       </c>
@@ -6647,7 +6652,7 @@
         <v>32.64</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -6666,7 +6671,7 @@
       <c r="G157">
         <v>346</v>
       </c>
-      <c r="H157" s="2">
+      <c r="H157">
         <v>15.44</v>
       </c>
       <c r="I157">
@@ -6674,7 +6679,7 @@
         <v>21.89</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -6693,7 +6698,7 @@
       <c r="G158">
         <v>346</v>
       </c>
-      <c r="H158" s="2">
+      <c r="H158">
         <v>16.73</v>
       </c>
       <c r="I158">
@@ -6701,7 +6706,7 @@
         <v>17.98</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -6720,7 +6725,7 @@
       <c r="G159">
         <v>346</v>
       </c>
-      <c r="H159" s="2">
+      <c r="H159">
         <v>30.58</v>
       </c>
       <c r="I159">
@@ -6728,7 +6733,7 @@
         <v>30.64</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -6747,7 +6752,7 @@
       <c r="G160">
         <v>346</v>
       </c>
-      <c r="H160" s="2">
+      <c r="H160">
         <v>35.950000000000003</v>
       </c>
       <c r="I160">
@@ -6755,7 +6760,7 @@
         <v>35.49</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -6774,7 +6779,7 @@
       <c r="G161">
         <v>346</v>
       </c>
-      <c r="H161" s="2">
+      <c r="H161">
         <v>16</v>
       </c>
       <c r="I161">
@@ -6782,7 +6787,7 @@
         <v>15.34</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -6809,7 +6814,7 @@
         <v>37.119999999999997</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -6836,7 +6841,7 @@
         <v>19.72</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -6863,7 +6868,7 @@
         <v>21.419999999999998</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -6890,7 +6895,7 @@
         <v>21.57</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -6917,7 +6922,7 @@
         <v>15.72</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>181</v>
       </c>
@@ -6944,7 +6949,7 @@
         <v>30.03</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>182</v>
       </c>
@@ -6971,7 +6976,7 @@
         <v>11.33</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>183</v>
       </c>
@@ -6998,7 +7003,7 @@
         <v>39.270000000000003</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>184</v>
       </c>
@@ -7025,7 +7030,7 @@
         <v>15.29</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>185</v>
       </c>
@@ -7052,7 +7057,7 @@
         <v>32.700000000000003</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>186</v>
       </c>
@@ -7079,7 +7084,7 @@
         <v>11.67</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>187</v>
       </c>
@@ -7106,7 +7111,7 @@
         <v>27.07</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>188</v>
       </c>
@@ -7133,7 +7138,7 @@
         <v>35.24</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>189</v>
       </c>
@@ -7160,7 +7165,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -7187,7 +7192,7 @@
         <v>27.62</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -7214,7 +7219,7 @@
         <v>14.48</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -7241,7 +7246,7 @@
         <v>14.75</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>193</v>
       </c>
@@ -7268,7 +7273,7 @@
         <v>19.309999999999999</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>194</v>
       </c>
@@ -7295,7 +7300,7 @@
         <v>19.18</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>195</v>
       </c>
@@ -7341,7 +7346,7 @@
       <c r="G182">
         <v>346</v>
       </c>
-      <c r="H182" s="2">
+      <c r="H182">
         <v>59.53</v>
       </c>
       <c r="I182">
@@ -7367,10 +7372,10 @@
       <c r="G183">
         <v>346</v>
       </c>
-      <c r="H183" s="2">
+      <c r="H183">
         <v>40.6</v>
       </c>
-      <c r="I183" s="2">
+      <c r="I183">
         <v>69.02</v>
       </c>
     </row>
@@ -7393,10 +7398,10 @@
       <c r="G184">
         <v>346</v>
       </c>
-      <c r="H184" s="2">
+      <c r="H184">
         <v>19.579999999999998</v>
       </c>
-      <c r="I184" s="2">
+      <c r="I184">
         <v>49.56</v>
       </c>
     </row>
@@ -7419,10 +7424,10 @@
       <c r="G185">
         <v>346</v>
       </c>
-      <c r="H185" s="2">
+      <c r="H185">
         <v>6.74</v>
       </c>
-      <c r="I185" s="2">
+      <c r="I185">
         <v>23.77</v>
       </c>
     </row>
@@ -7445,10 +7450,10 @@
       <c r="G186">
         <v>346</v>
       </c>
-      <c r="H186" s="2">
+      <c r="H186">
         <v>34.5</v>
       </c>
-      <c r="I186" s="2">
+      <c r="I186">
         <v>54.95</v>
       </c>
     </row>
@@ -9501,11 +9506,11 @@
       <c r="E272" t="s">
         <v>290</v>
       </c>
-      <c r="G272" s="3">
+      <c r="G272" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="273" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>291</v>
       </c>
@@ -9521,11 +9526,11 @@
       <c r="E273" t="s">
         <v>290</v>
       </c>
-      <c r="G273" s="3">
+      <c r="G273" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="274" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>292</v>
       </c>
@@ -9541,11 +9546,11 @@
       <c r="E274" t="s">
         <v>290</v>
       </c>
-      <c r="G274" s="3">
+      <c r="G274" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="275" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>293</v>
       </c>
@@ -9561,11 +9566,11 @@
       <c r="E275" t="s">
         <v>290</v>
       </c>
-      <c r="G275" s="3">
+      <c r="G275" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="276" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>294</v>
       </c>
@@ -9581,11 +9586,11 @@
       <c r="E276" t="s">
         <v>290</v>
       </c>
-      <c r="G276" s="3">
+      <c r="G276" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="277" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>295</v>
       </c>
@@ -9601,8 +9606,17 @@
       <c r="E277" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="278" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G277">
+        <v>349</v>
+      </c>
+      <c r="H277">
+        <v>7.65</v>
+      </c>
+      <c r="I277">
+        <v>4.6399999999999997</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>296</v>
       </c>
@@ -9618,8 +9632,17 @@
       <c r="E278" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="279" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G278">
+        <v>349</v>
+      </c>
+      <c r="H278">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="I278">
+        <v>8.91</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>297</v>
       </c>
@@ -9635,8 +9658,17 @@
       <c r="E279" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="280" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G279">
+        <v>349</v>
+      </c>
+      <c r="H279">
+        <v>12.46</v>
+      </c>
+      <c r="I279">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>298</v>
       </c>
@@ -9652,8 +9684,17 @@
       <c r="E280" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="281" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G280">
+        <v>349</v>
+      </c>
+      <c r="H280">
+        <v>9.85</v>
+      </c>
+      <c r="I280">
+        <v>9.02</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>299</v>
       </c>
@@ -9669,8 +9710,17 @@
       <c r="E281" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="282" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G281">
+        <v>349</v>
+      </c>
+      <c r="H281">
+        <v>15.35</v>
+      </c>
+      <c r="I281">
+        <v>11.44</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>300</v>
       </c>
@@ -9686,8 +9736,17 @@
       <c r="E282" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="283" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G282">
+        <v>349</v>
+      </c>
+      <c r="H282">
+        <v>6.28</v>
+      </c>
+      <c r="I282">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>301</v>
       </c>
@@ -9703,8 +9762,17 @@
       <c r="E283" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="284" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G283">
+        <v>349</v>
+      </c>
+      <c r="H283">
+        <v>10.18</v>
+      </c>
+      <c r="I283">
+        <v>7.71</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>302</v>
       </c>
@@ -9720,8 +9788,17 @@
       <c r="E284" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="285" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G284">
+        <v>349</v>
+      </c>
+      <c r="H284" s="1">
+        <v>6.95</v>
+      </c>
+      <c r="I284" s="3">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>303</v>
       </c>
@@ -9737,8 +9814,17 @@
       <c r="E285" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="286" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G285">
+        <v>349</v>
+      </c>
+      <c r="H285">
+        <v>14.54</v>
+      </c>
+      <c r="I285">
+        <v>12.16</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>304</v>
       </c>
@@ -9754,11 +9840,11 @@
       <c r="E286" t="s">
         <v>290</v>
       </c>
-      <c r="G286" s="3">
+      <c r="G286" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="287" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>305</v>
       </c>
@@ -9774,11 +9860,11 @@
       <c r="E287" t="s">
         <v>290</v>
       </c>
-      <c r="G287" s="3">
+      <c r="G287" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="288" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>306</v>
       </c>
@@ -9794,11 +9880,11 @@
       <c r="E288" t="s">
         <v>290</v>
       </c>
-      <c r="G288" s="3">
+      <c r="G288" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="289" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>307</v>
       </c>
@@ -9814,11 +9900,11 @@
       <c r="E289" t="s">
         <v>290</v>
       </c>
-      <c r="G289" s="3">
+      <c r="G289" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="290" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>308</v>
       </c>
@@ -9834,11 +9920,11 @@
       <c r="E290" t="s">
         <v>290</v>
       </c>
-      <c r="G290" s="3">
+      <c r="G290" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="291" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>309</v>
       </c>
@@ -9854,8 +9940,17 @@
       <c r="E291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G291">
+        <v>349</v>
+      </c>
+      <c r="H291">
+        <v>11.04</v>
+      </c>
+      <c r="I291">
+        <v>12.31</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>310</v>
       </c>
@@ -9871,8 +9966,17 @@
       <c r="E292" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="293" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G292">
+        <v>349</v>
+      </c>
+      <c r="H292">
+        <v>15.63</v>
+      </c>
+      <c r="I292">
+        <v>22.69</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>311</v>
       </c>
@@ -9888,8 +9992,17 @@
       <c r="E293" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="294" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G293">
+        <v>349</v>
+      </c>
+      <c r="H293">
+        <v>9.83</v>
+      </c>
+      <c r="I293">
+        <v>11.66</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>312</v>
       </c>
@@ -9905,8 +10018,17 @@
       <c r="E294" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="295" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G294">
+        <v>349</v>
+      </c>
+      <c r="H294">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="I294">
+        <v>11.08</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>313</v>
       </c>
@@ -9922,8 +10044,17 @@
       <c r="E295" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="296" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G295">
+        <v>349</v>
+      </c>
+      <c r="H295">
+        <v>21.18</v>
+      </c>
+      <c r="I295">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
@@ -9939,8 +10070,17 @@
       <c r="E296" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="297" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G296">
+        <v>349</v>
+      </c>
+      <c r="H296">
+        <v>14.4</v>
+      </c>
+      <c r="I296">
+        <v>11.15</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
@@ -9956,8 +10096,17 @@
       <c r="E297" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="298" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G297">
+        <v>349</v>
+      </c>
+      <c r="H297">
+        <v>17.88</v>
+      </c>
+      <c r="I297">
+        <v>15.08</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
@@ -9973,8 +10122,17 @@
       <c r="E298" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="299" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G298">
+        <v>349</v>
+      </c>
+      <c r="H298">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="I298">
+        <v>9.82</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
@@ -9990,8 +10148,17 @@
       <c r="E299" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="300" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G299">
+        <v>349</v>
+      </c>
+      <c r="H299">
+        <v>11.17</v>
+      </c>
+      <c r="I299">
+        <v>10.07</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -10007,8 +10174,17 @@
       <c r="E300" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="301" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G300">
+        <v>349</v>
+      </c>
+      <c r="H300">
+        <v>11.15</v>
+      </c>
+      <c r="I300">
+        <v>12.38</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>319</v>
       </c>
@@ -10024,11 +10200,11 @@
       <c r="E301" t="s">
         <v>290</v>
       </c>
-      <c r="G301" s="3">
+      <c r="G301" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="302" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>320</v>
       </c>
@@ -10044,11 +10220,11 @@
       <c r="E302" t="s">
         <v>290</v>
       </c>
-      <c r="G302" s="3">
+      <c r="G302" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="303" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>321</v>
       </c>
@@ -10064,11 +10240,11 @@
       <c r="E303" t="s">
         <v>290</v>
       </c>
-      <c r="G303" s="3">
+      <c r="G303" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="304" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>322</v>
       </c>
@@ -10084,11 +10260,11 @@
       <c r="E304" t="s">
         <v>290</v>
       </c>
-      <c r="G304" s="3">
+      <c r="G304" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="305" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>323</v>
       </c>
@@ -10104,11 +10280,11 @@
       <c r="E305" t="s">
         <v>290</v>
       </c>
-      <c r="G305" s="3">
+      <c r="G305" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="306" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>324</v>
       </c>
@@ -10124,8 +10300,17 @@
       <c r="E306" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="307" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G306">
+        <v>349</v>
+      </c>
+      <c r="H306">
+        <v>10.98</v>
+      </c>
+      <c r="I306">
+        <v>11.42</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>325</v>
       </c>
@@ -10141,8 +10326,17 @@
       <c r="E307" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="308" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G307">
+        <v>349</v>
+      </c>
+      <c r="H307">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="I307">
+        <v>15.25</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>326</v>
       </c>
@@ -10158,8 +10352,17 @@
       <c r="E308" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="309" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G308">
+        <v>349</v>
+      </c>
+      <c r="H308">
+        <v>8.15</v>
+      </c>
+      <c r="I308">
+        <v>12.47</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>327</v>
       </c>
@@ -10175,8 +10378,17 @@
       <c r="E309" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="310" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G309">
+        <v>349</v>
+      </c>
+      <c r="H309">
+        <v>11.08</v>
+      </c>
+      <c r="I309">
+        <v>21.88</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>328</v>
       </c>
@@ -10192,8 +10404,17 @@
       <c r="E310" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="311" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G310">
+        <v>349</v>
+      </c>
+      <c r="H310">
+        <v>12.13</v>
+      </c>
+      <c r="I310">
+        <v>11.14</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>329</v>
       </c>
@@ -10209,8 +10430,17 @@
       <c r="E311" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="312" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G311">
+        <v>349</v>
+      </c>
+      <c r="H311">
+        <v>14.33</v>
+      </c>
+      <c r="I311">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>330</v>
       </c>
@@ -10226,8 +10456,17 @@
       <c r="E312" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="313" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G312">
+        <v>349</v>
+      </c>
+      <c r="H312">
+        <v>19.16</v>
+      </c>
+      <c r="I312">
+        <v>16.02</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>331</v>
       </c>
@@ -10243,8 +10482,17 @@
       <c r="E313" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="314" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G313">
+        <v>349</v>
+      </c>
+      <c r="H313">
+        <v>10.35</v>
+      </c>
+      <c r="I313">
+        <v>12.55</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>332</v>
       </c>
@@ -10260,8 +10508,17 @@
       <c r="E314" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="315" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G314">
+        <v>349</v>
+      </c>
+      <c r="H314">
+        <v>17.91</v>
+      </c>
+      <c r="I314">
+        <v>21.47</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>333</v>
       </c>
@@ -10277,8 +10534,17 @@
       <c r="E315" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="316" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G315">
+        <v>349</v>
+      </c>
+      <c r="H315">
+        <v>10.6</v>
+      </c>
+      <c r="I315">
+        <v>13.79</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>334</v>
       </c>
@@ -10294,11 +10560,11 @@
       <c r="E316" t="s">
         <v>290</v>
       </c>
-      <c r="G316" s="3">
+      <c r="G316" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="317" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>335</v>
       </c>
@@ -10314,11 +10580,11 @@
       <c r="E317" t="s">
         <v>290</v>
       </c>
-      <c r="G317" s="3">
+      <c r="G317" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="318" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>336</v>
       </c>
@@ -10334,11 +10600,11 @@
       <c r="E318" t="s">
         <v>290</v>
       </c>
-      <c r="G318" s="3">
+      <c r="G318" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="319" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>337</v>
       </c>
@@ -10354,11 +10620,11 @@
       <c r="E319" t="s">
         <v>290</v>
       </c>
-      <c r="G319" s="3">
+      <c r="G319" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="320" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>338</v>
       </c>
@@ -10374,11 +10640,11 @@
       <c r="E320" t="s">
         <v>290</v>
       </c>
-      <c r="G320" s="3">
+      <c r="G320" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="321" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>339</v>
       </c>
@@ -10394,8 +10660,17 @@
       <c r="E321" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="322" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G321">
+        <v>349</v>
+      </c>
+      <c r="H321">
+        <v>18.52</v>
+      </c>
+      <c r="I321">
+        <v>18.829999999999998</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>340</v>
       </c>
@@ -10411,8 +10686,17 @@
       <c r="E322" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="323" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G322">
+        <v>349</v>
+      </c>
+      <c r="H322">
+        <v>15.15</v>
+      </c>
+      <c r="I322">
+        <v>8.6300000000000008</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>341</v>
       </c>
@@ -10428,8 +10712,17 @@
       <c r="E323" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="324" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G323">
+        <v>349</v>
+      </c>
+      <c r="H323">
+        <v>13.35</v>
+      </c>
+      <c r="I323">
+        <v>12.49</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>342</v>
       </c>
@@ -10445,8 +10738,17 @@
       <c r="E324" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="325" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G324">
+        <v>349</v>
+      </c>
+      <c r="H324">
+        <v>8.02</v>
+      </c>
+      <c r="I324">
+        <v>7.75</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -10462,8 +10764,17 @@
       <c r="E325" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="326" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G325">
+        <v>349</v>
+      </c>
+      <c r="H325">
+        <v>17.350000000000001</v>
+      </c>
+      <c r="I325">
+        <v>14.85</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>344</v>
       </c>
@@ -10479,8 +10790,17 @@
       <c r="E326" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="327" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G326">
+        <v>349</v>
+      </c>
+      <c r="H326">
+        <v>11.02</v>
+      </c>
+      <c r="I326">
+        <v>10.54</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>345</v>
       </c>
@@ -10496,8 +10816,17 @@
       <c r="E327" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="328" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G327">
+        <v>349</v>
+      </c>
+      <c r="H327">
+        <v>13.14</v>
+      </c>
+      <c r="I327">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>346</v>
       </c>
@@ -10513,8 +10842,17 @@
       <c r="E328" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="329" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G328">
+        <v>349</v>
+      </c>
+      <c r="H328">
+        <v>10.69</v>
+      </c>
+      <c r="I328">
+        <v>13.76</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>347</v>
       </c>
@@ -10530,11 +10868,11 @@
       <c r="E329" t="s">
         <v>290</v>
       </c>
-      <c r="G329" s="3">
+      <c r="G329" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="330" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>348</v>
       </c>
@@ -10550,11 +10888,11 @@
       <c r="E330" t="s">
         <v>290</v>
       </c>
-      <c r="G330" s="3">
+      <c r="G330" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="331" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>349</v>
       </c>
@@ -10570,11 +10908,11 @@
       <c r="E331" t="s">
         <v>290</v>
       </c>
-      <c r="G331" s="3">
+      <c r="G331" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="332" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>350</v>
       </c>
@@ -10590,11 +10928,11 @@
       <c r="E332" t="s">
         <v>290</v>
       </c>
-      <c r="G332" s="3">
+      <c r="G332" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="333" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>351</v>
       </c>
@@ -10610,11 +10948,11 @@
       <c r="E333" t="s">
         <v>290</v>
       </c>
-      <c r="G333" s="3">
+      <c r="G333" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="334" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>352</v>
       </c>
@@ -10630,8 +10968,17 @@
       <c r="E334" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="335" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G334">
+        <v>349</v>
+      </c>
+      <c r="H334">
+        <v>15.89</v>
+      </c>
+      <c r="I334">
+        <v>23.02</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>353</v>
       </c>
@@ -10647,8 +10994,17 @@
       <c r="E335" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="336" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G335">
+        <v>349</v>
+      </c>
+      <c r="H335">
+        <v>10.25</v>
+      </c>
+      <c r="I335">
+        <v>12.47</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>354</v>
       </c>
@@ -10664,8 +11020,17 @@
       <c r="E336" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="337" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G336">
+        <v>349</v>
+      </c>
+      <c r="H336">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="I336">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>355</v>
       </c>
@@ -10681,8 +11046,17 @@
       <c r="E337" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="338" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G337">
+        <v>349</v>
+      </c>
+      <c r="H337">
+        <v>15.03</v>
+      </c>
+      <c r="I337">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>356</v>
       </c>
@@ -10698,8 +11072,17 @@
       <c r="E338" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="339" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G338">
+        <v>349</v>
+      </c>
+      <c r="H338">
+        <v>12.54</v>
+      </c>
+      <c r="I338">
+        <v>16.62</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>357</v>
       </c>
@@ -10715,8 +11098,17 @@
       <c r="E339" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="340" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G339">
+        <v>349</v>
+      </c>
+      <c r="H339">
+        <v>11.25</v>
+      </c>
+      <c r="I339">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>358</v>
       </c>
@@ -10732,8 +11124,17 @@
       <c r="E340" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="341" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G340">
+        <v>349</v>
+      </c>
+      <c r="H340">
+        <v>8.26</v>
+      </c>
+      <c r="I340">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>359</v>
       </c>
@@ -10749,8 +11150,17 @@
       <c r="E341" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="342" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G341">
+        <v>349</v>
+      </c>
+      <c r="H341">
+        <v>10.84</v>
+      </c>
+      <c r="I341">
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>360</v>
       </c>
@@ -10766,8 +11176,17 @@
       <c r="E342" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="343" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G342">
+        <v>349</v>
+      </c>
+      <c r="H342">
+        <v>10.98</v>
+      </c>
+      <c r="I342">
+        <v>10.32</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>361</v>
       </c>
@@ -10783,8 +11202,17 @@
       <c r="E343" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="344" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G343">
+        <v>349</v>
+      </c>
+      <c r="H343">
+        <v>10.46</v>
+      </c>
+      <c r="I343">
+        <v>8.85</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -10800,11 +11228,11 @@
       <c r="E344" t="s">
         <v>290</v>
       </c>
-      <c r="G344" s="3">
+      <c r="G344" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="345" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>363</v>
       </c>
@@ -10820,11 +11248,11 @@
       <c r="E345" t="s">
         <v>290</v>
       </c>
-      <c r="G345" s="3">
+      <c r="G345" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="346" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>364</v>
       </c>
@@ -10840,11 +11268,11 @@
       <c r="E346" t="s">
         <v>290</v>
       </c>
-      <c r="G346" s="3">
+      <c r="G346" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="347" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>365</v>
       </c>
@@ -10860,11 +11288,11 @@
       <c r="E347" t="s">
         <v>290</v>
       </c>
-      <c r="G347" s="3">
+      <c r="G347" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="348" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>366</v>
       </c>
@@ -10880,11 +11308,11 @@
       <c r="E348" t="s">
         <v>290</v>
       </c>
-      <c r="G348" s="3">
+      <c r="G348" s="2">
         <v>346</v>
       </c>
     </row>
-    <row r="349" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>367</v>
       </c>
@@ -10900,8 +11328,17 @@
       <c r="E349" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="350" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G349">
+        <v>349</v>
+      </c>
+      <c r="H349">
+        <v>14.67</v>
+      </c>
+      <c r="I349">
+        <v>24.81</v>
+      </c>
+    </row>
+    <row r="350" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>368</v>
       </c>
@@ -10917,8 +11354,17 @@
       <c r="E350" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="351" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G350">
+        <v>349</v>
+      </c>
+      <c r="H350">
+        <v>10.19</v>
+      </c>
+      <c r="I350">
+        <v>24.56</v>
+      </c>
+    </row>
+    <row r="351" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>369</v>
       </c>
@@ -10934,8 +11380,17 @@
       <c r="E351" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="352" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G351">
+        <v>349</v>
+      </c>
+      <c r="H351">
+        <v>10.25</v>
+      </c>
+      <c r="I351">
+        <v>16.96</v>
+      </c>
+    </row>
+    <row r="352" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>370</v>
       </c>
@@ -10950,6 +11405,15 @@
       </c>
       <c r="E352" t="s">
         <v>290</v>
+      </c>
+      <c r="G352">
+        <v>349</v>
+      </c>
+      <c r="H352">
+        <v>8.75</v>
+      </c>
+      <c r="I352">
+        <v>16.36</v>
       </c>
     </row>
     <row r="353" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -10968,6 +11432,15 @@
       <c r="E353" t="s">
         <v>290</v>
       </c>
+      <c r="G353">
+        <v>349</v>
+      </c>
+      <c r="H353">
+        <v>14.38</v>
+      </c>
+      <c r="I353">
+        <v>19.04</v>
+      </c>
     </row>
     <row r="354" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
@@ -10985,6 +11458,15 @@
       <c r="E354" t="s">
         <v>290</v>
       </c>
+      <c r="G354">
+        <v>349</v>
+      </c>
+      <c r="H354">
+        <v>14.69</v>
+      </c>
+      <c r="I354" s="1">
+        <v>18.309999999999999</v>
+      </c>
     </row>
     <row r="355" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
@@ -11002,6 +11484,15 @@
       <c r="E355" t="s">
         <v>290</v>
       </c>
+      <c r="G355">
+        <v>349</v>
+      </c>
+      <c r="H355">
+        <v>14.54</v>
+      </c>
+      <c r="I355">
+        <v>14.84</v>
+      </c>
     </row>
     <row r="356" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
@@ -11019,6 +11510,15 @@
       <c r="E356" t="s">
         <v>290</v>
       </c>
+      <c r="G356">
+        <v>349</v>
+      </c>
+      <c r="H356">
+        <v>19.82</v>
+      </c>
+      <c r="I356">
+        <v>14.42</v>
+      </c>
     </row>
     <row r="357" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
@@ -11035,6 +11535,15 @@
       </c>
       <c r="E357" t="s">
         <v>290</v>
+      </c>
+      <c r="G357">
+        <v>349</v>
+      </c>
+      <c r="H357">
+        <v>15.18</v>
+      </c>
+      <c r="I357">
+        <v>18.93</v>
       </c>
     </row>
     <row r="358" spans="1:9" hidden="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
re-added poba bloc 1 that got lost in translation in december and recovered from old commit
</commit_message>
<xml_diff>
--- a/data/treeMeasurements/biomass.xlsx
+++ b/data/treeMeasurements/biomass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/github/fuelinex/data/treeMeasurements/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D3FECD-7BDB-8F4C-BFFD-E5C956E3811D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB71FB-E238-2744-9A66-B367B35C3BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shoot_elongation" sheetId="1" r:id="rId1"/>
@@ -2036,11 +2036,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2116,7 +2115,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1260360</xdr:colOff>
-      <xdr:row>276</xdr:row>
+      <xdr:row>271</xdr:row>
       <xdr:rowOff>10414</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -2204,11 +2203,6 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I617" totalsRowShown="0">
   <autoFilter ref="A1:I617" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="4">
       <filters>
         <filter val="populus_balsamifera"/>
@@ -2510,9 +2504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J617"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H352" sqref="H352"/>
+    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="187" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G296" sqref="G296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9490,7 +9484,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>288</v>
       </c>
@@ -9509,8 +9503,14 @@
       <c r="G272" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H272">
+        <v>9.57</v>
+      </c>
+      <c r="I272">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>291</v>
       </c>
@@ -9529,8 +9529,14 @@
       <c r="G273" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H273">
+        <v>10.09</v>
+      </c>
+      <c r="I273">
+        <v>19.350000000000001</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>292</v>
       </c>
@@ -9549,8 +9555,14 @@
       <c r="G274" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H274">
+        <v>10.53</v>
+      </c>
+      <c r="I274">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>293</v>
       </c>
@@ -9569,8 +9581,14 @@
       <c r="G275" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H275">
+        <v>11.77</v>
+      </c>
+      <c r="I275">
+        <v>11.75</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>294</v>
       </c>
@@ -9588,6 +9606,12 @@
       </c>
       <c r="G276" s="2">
         <v>346</v>
+      </c>
+      <c r="H276">
+        <v>13.65</v>
+      </c>
+      <c r="I276">
+        <v>11.79</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.2">
@@ -9720,7 +9744,7 @@
         <v>11.44</v>
       </c>
     </row>
-    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>300</v>
       </c>
@@ -9746,7 +9770,7 @@
         <v>5.26</v>
       </c>
     </row>
-    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>301</v>
       </c>
@@ -9772,7 +9796,7 @@
         <v>7.71</v>
       </c>
     </row>
-    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>302</v>
       </c>
@@ -9794,11 +9818,11 @@
       <c r="H284" s="1">
         <v>6.95</v>
       </c>
-      <c r="I284" s="3">
+      <c r="I284">
         <v>8.19</v>
       </c>
     </row>
-    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>303</v>
       </c>
@@ -9824,7 +9848,7 @@
         <v>12.16</v>
       </c>
     </row>
-    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>304</v>
       </c>
@@ -9843,8 +9867,14 @@
       <c r="G286" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H286">
+        <v>11.76</v>
+      </c>
+      <c r="I286">
+        <v>12.07</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>305</v>
       </c>
@@ -9863,8 +9893,14 @@
       <c r="G287" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H287">
+        <v>11.12</v>
+      </c>
+      <c r="I287">
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>306</v>
       </c>
@@ -9883,8 +9919,14 @@
       <c r="G288" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H288">
+        <v>10.1</v>
+      </c>
+      <c r="I288">
+        <v>13.71</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>307</v>
       </c>
@@ -9903,8 +9945,14 @@
       <c r="G289" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H289">
+        <v>15.78</v>
+      </c>
+      <c r="I289">
+        <v>17.809999999999999</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>308</v>
       </c>
@@ -9922,6 +9970,12 @@
       </c>
       <c r="G290" s="2">
         <v>346</v>
+      </c>
+      <c r="H290">
+        <v>11.58</v>
+      </c>
+      <c r="I290">
+        <v>16.670000000000002</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.2">
@@ -10054,7 +10108,7 @@
         <v>18.7</v>
       </c>
     </row>
-    <row r="296" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>314</v>
       </c>
@@ -10080,7 +10134,7 @@
         <v>11.15</v>
       </c>
     </row>
-    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>315</v>
       </c>
@@ -10106,7 +10160,7 @@
         <v>15.08</v>
       </c>
     </row>
-    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>316</v>
       </c>
@@ -10132,7 +10186,7 @@
         <v>9.82</v>
       </c>
     </row>
-    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>317</v>
       </c>
@@ -10158,7 +10212,7 @@
         <v>10.07</v>
       </c>
     </row>
-    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>318</v>
       </c>
@@ -10184,7 +10238,7 @@
         <v>12.38</v>
       </c>
     </row>
-    <row r="301" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>319</v>
       </c>
@@ -10203,8 +10257,14 @@
       <c r="G301" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="302" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H301">
+        <v>10.119999999999999</v>
+      </c>
+      <c r="I301">
+        <v>17.36</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>320</v>
       </c>
@@ -10223,8 +10283,14 @@
       <c r="G302" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="303" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H302">
+        <v>9.86</v>
+      </c>
+      <c r="I302">
+        <v>16.41</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>321</v>
       </c>
@@ -10243,8 +10309,14 @@
       <c r="G303" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H303">
+        <v>9.74</v>
+      </c>
+      <c r="I303">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>322</v>
       </c>
@@ -10263,8 +10335,14 @@
       <c r="G304" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H304">
+        <v>12.18</v>
+      </c>
+      <c r="I304">
+        <v>16.28</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>323</v>
       </c>
@@ -10282,6 +10360,12 @@
       </c>
       <c r="G305" s="2">
         <v>346</v>
+      </c>
+      <c r="H305">
+        <v>12.94</v>
+      </c>
+      <c r="I305">
+        <v>16.43</v>
       </c>
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.2">
@@ -10414,7 +10498,7 @@
         <v>11.14</v>
       </c>
     </row>
-    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>329</v>
       </c>
@@ -10440,7 +10524,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>330</v>
       </c>
@@ -10466,7 +10550,7 @@
         <v>16.02</v>
       </c>
     </row>
-    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>331</v>
       </c>
@@ -10492,7 +10576,7 @@
         <v>12.55</v>
       </c>
     </row>
-    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>332</v>
       </c>
@@ -10518,7 +10602,7 @@
         <v>21.47</v>
       </c>
     </row>
-    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>333</v>
       </c>
@@ -10544,7 +10628,7 @@
         <v>13.79</v>
       </c>
     </row>
-    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>334</v>
       </c>
@@ -10563,8 +10647,14 @@
       <c r="G316" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H316">
+        <v>14.64</v>
+      </c>
+      <c r="I316">
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>335</v>
       </c>
@@ -10583,8 +10673,14 @@
       <c r="G317" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H317">
+        <v>10.19</v>
+      </c>
+      <c r="I317">
+        <v>21.84</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>336</v>
       </c>
@@ -10603,8 +10699,14 @@
       <c r="G318" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H318">
+        <v>11.07</v>
+      </c>
+      <c r="I318">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>337</v>
       </c>
@@ -10623,8 +10725,14 @@
       <c r="G319" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H319">
+        <v>13.82</v>
+      </c>
+      <c r="I319">
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>338</v>
       </c>
@@ -10642,6 +10750,12 @@
       </c>
       <c r="G320" s="2">
         <v>346</v>
+      </c>
+      <c r="H320">
+        <v>8.33</v>
+      </c>
+      <c r="I320">
+        <v>7.52</v>
       </c>
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.2">
@@ -10722,7 +10836,7 @@
         <v>12.49</v>
       </c>
     </row>
-    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>342</v>
       </c>
@@ -10748,7 +10862,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>343</v>
       </c>
@@ -10774,7 +10888,7 @@
         <v>14.85</v>
       </c>
     </row>
-    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>344</v>
       </c>
@@ -10800,7 +10914,7 @@
         <v>10.54</v>
       </c>
     </row>
-    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>345</v>
       </c>
@@ -10826,7 +10940,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>346</v>
       </c>
@@ -10852,7 +10966,7 @@
         <v>13.76</v>
       </c>
     </row>
-    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>347</v>
       </c>
@@ -10871,8 +10985,14 @@
       <c r="G329" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H329">
+        <v>13.46</v>
+      </c>
+      <c r="I329">
+        <v>18.649999999999999</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>348</v>
       </c>
@@ -10891,8 +11011,14 @@
       <c r="G330" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H330">
+        <v>13.07</v>
+      </c>
+      <c r="I330">
+        <v>19.38</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>349</v>
       </c>
@@ -10911,8 +11037,14 @@
       <c r="G331" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H331">
+        <v>10.17</v>
+      </c>
+      <c r="I331">
+        <v>16.88</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>350</v>
       </c>
@@ -10931,8 +11063,14 @@
       <c r="G332" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H332">
+        <v>11.59</v>
+      </c>
+      <c r="I332">
+        <v>21.49</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>351</v>
       </c>
@@ -10950,6 +11088,12 @@
       </c>
       <c r="G333" s="2">
         <v>346</v>
+      </c>
+      <c r="H333">
+        <v>16.16</v>
+      </c>
+      <c r="I333">
+        <v>23.58</v>
       </c>
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.2">
@@ -11082,7 +11226,7 @@
         <v>16.62</v>
       </c>
     </row>
-    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>357</v>
       </c>
@@ -11108,7 +11252,7 @@
         <v>11.75</v>
       </c>
     </row>
-    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>358</v>
       </c>
@@ -11134,7 +11278,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>359</v>
       </c>
@@ -11160,7 +11304,7 @@
         <v>9.14</v>
       </c>
     </row>
-    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>360</v>
       </c>
@@ -11186,7 +11330,7 @@
         <v>10.32</v>
       </c>
     </row>
-    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>361</v>
       </c>
@@ -11212,7 +11356,7 @@
         <v>8.85</v>
       </c>
     </row>
-    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>362</v>
       </c>
@@ -11231,8 +11375,14 @@
       <c r="G344" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H344">
+        <v>13.77</v>
+      </c>
+      <c r="I344">
+        <v>25.03</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>363</v>
       </c>
@@ -11251,8 +11401,14 @@
       <c r="G345" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H345">
+        <v>12.79</v>
+      </c>
+      <c r="I345">
+        <v>14.93</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>364</v>
       </c>
@@ -11271,8 +11427,14 @@
       <c r="G346" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="347" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H346">
+        <v>12.13</v>
+      </c>
+      <c r="I346">
+        <v>15.69</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>365</v>
       </c>
@@ -11291,8 +11453,14 @@
       <c r="G347" s="2">
         <v>346</v>
       </c>
-    </row>
-    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H347">
+        <v>6.75</v>
+      </c>
+      <c r="I347">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>366</v>
       </c>
@@ -11310,6 +11478,12 @@
       </c>
       <c r="G348" s="2">
         <v>346</v>
+      </c>
+      <c r="H348">
+        <v>12.96</v>
+      </c>
+      <c r="I348">
+        <v>11.95</v>
       </c>
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.2">
@@ -11416,7 +11590,7 @@
         <v>16.36</v>
       </c>
     </row>
-    <row r="353" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>371</v>
       </c>
@@ -11442,7 +11616,7 @@
         <v>19.04</v>
       </c>
     </row>
-    <row r="354" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>372</v>
       </c>
@@ -11468,7 +11642,7 @@
         <v>18.309999999999999</v>
       </c>
     </row>
-    <row r="355" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>373</v>
       </c>
@@ -11494,7 +11668,7 @@
         <v>14.84</v>
       </c>
     </row>
-    <row r="356" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>374</v>
       </c>
@@ -11520,7 +11694,7 @@
         <v>14.42</v>
       </c>
     </row>
-    <row r="357" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>375</v>
       </c>

</xml_diff>